<commit_message>
11s2 2023 & 4s2 2024
</commit_message>
<xml_diff>
--- a/Allen_Dark_Analysis.xlsx
+++ b/Allen_Dark_Analysis.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\CompSciFinal\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586E515B-E01A-46B9-9570-D170D19ACEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -142,6 +136,12 @@
     <t>test12.mhtml</t>
   </si>
   <si>
+    <t>test13.mht</t>
+  </si>
+  <si>
+    <t>test14.mht</t>
+  </si>
+  <si>
     <t>JEE MAINS 24 Jan Shift 1 | 27th Dec,2024 | Online Mode</t>
   </si>
   <si>
@@ -187,6 +187,12 @@
     <t>JEE MAINS 11 April Shift 1 | 2nd Dec,2025 | Online Mode</t>
   </si>
   <si>
+    <t>JEE MAINS 11 April Shift 2 | 2nd Dec,2025 | Online Mode</t>
+  </si>
+  <si>
+    <t>JEE MAINS 04 Apr Shift 2 | 10th Dec,2024 | Online Mode</t>
+  </si>
+  <si>
     <t>6015 to 6181</t>
   </si>
   <si>
@@ -227,13 +233,16 @@
   </si>
   <si>
     <t>2963 to 3105</t>
+  </si>
+  <si>
+    <t>131 to 151</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,21 +279,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -322,7 +323,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -356,7 +357,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -391,10 +391,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -567,42 +566,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" customWidth="1"/>
-    <col min="24" max="24" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" customWidth="1"/>
+    <col min="18" max="21" width="10.7109375" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" customWidth="1"/>
+    <col min="23" max="25" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -679,12 +665,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="B2" t="s">
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>193</v>
@@ -693,10 +679,10 @@
         <v>96</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G2">
-        <v>77.611940298507463</v>
+        <v>77.61194029850746</v>
       </c>
       <c r="H2">
         <v>52</v>
@@ -711,7 +697,7 @@
         <v>67</v>
       </c>
       <c r="L2">
-        <v>78.260869565217391</v>
+        <v>78.26086956521739</v>
       </c>
       <c r="M2">
         <v>18</v>
@@ -726,7 +712,7 @@
         <v>63</v>
       </c>
       <c r="Q2">
-        <v>77.272727272727266</v>
+        <v>77.27272727272727</v>
       </c>
       <c r="R2">
         <v>17</v>
@@ -741,7 +727,7 @@
         <v>63</v>
       </c>
       <c r="V2">
-        <v>77.272727272727266</v>
+        <v>77.27272727272727</v>
       </c>
       <c r="W2">
         <v>17</v>
@@ -753,12 +739,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>178</v>
@@ -767,7 +753,7 @@
         <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G3">
         <v>77.41935483870968</v>
@@ -815,7 +801,7 @@
         <v>48</v>
       </c>
       <c r="V3">
-        <v>76.470588235294116</v>
+        <v>76.47058823529412</v>
       </c>
       <c r="W3">
         <v>13</v>
@@ -827,12 +813,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="B4" t="s">
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>155</v>
@@ -841,10 +827,10 @@
         <v>91</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G4">
-        <v>71.666666666666671</v>
+        <v>71.66666666666667</v>
       </c>
       <c r="H4">
         <v>43</v>
@@ -874,7 +860,7 @@
         <v>44</v>
       </c>
       <c r="Q4">
-        <v>61.904761904761912</v>
+        <v>61.90476190476191</v>
       </c>
       <c r="R4">
         <v>13</v>
@@ -889,7 +875,7 @@
         <v>41</v>
       </c>
       <c r="V4">
-        <v>63.157894736842103</v>
+        <v>63.1578947368421</v>
       </c>
       <c r="W4">
         <v>12</v>
@@ -901,12 +887,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" t="s">
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>164</v>
@@ -915,10 +901,10 @@
         <v>93</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G5">
-        <v>69.696969696969703</v>
+        <v>69.6969696969697</v>
       </c>
       <c r="H5">
         <v>46</v>
@@ -933,7 +919,7 @@
         <v>71</v>
       </c>
       <c r="L5">
-        <v>79.166666666666657</v>
+        <v>79.16666666666666</v>
       </c>
       <c r="M5">
         <v>19</v>
@@ -948,7 +934,7 @@
         <v>43</v>
       </c>
       <c r="Q5">
-        <v>59.090909090909093</v>
+        <v>59.09090909090909</v>
       </c>
       <c r="R5">
         <v>13</v>
@@ -975,12 +961,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" t="s">
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D6">
         <v>222</v>
@@ -989,10 +975,10 @@
         <v>98</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G6">
-        <v>85.294117647058826</v>
+        <v>85.29411764705883</v>
       </c>
       <c r="H6">
         <v>58</v>
@@ -1022,7 +1008,7 @@
         <v>78</v>
       </c>
       <c r="Q6">
-        <v>90.909090909090907</v>
+        <v>90.90909090909091</v>
       </c>
       <c r="R6">
         <v>20</v>
@@ -1037,7 +1023,7 @@
         <v>82</v>
       </c>
       <c r="V6">
-        <v>91.304347826086953</v>
+        <v>91.30434782608695</v>
       </c>
       <c r="W6">
         <v>21</v>
@@ -1049,12 +1035,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" t="s">
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D7">
         <v>210</v>
@@ -1063,10 +1049,10 @@
         <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G7">
-        <v>84.615384615384613</v>
+        <v>84.61538461538461</v>
       </c>
       <c r="H7">
         <v>55</v>
@@ -1081,7 +1067,7 @@
         <v>71</v>
       </c>
       <c r="L7">
-        <v>79.166666666666657</v>
+        <v>79.16666666666666</v>
       </c>
       <c r="M7">
         <v>19</v>
@@ -1096,7 +1082,7 @@
         <v>71</v>
       </c>
       <c r="Q7">
-        <v>79.166666666666657</v>
+        <v>79.16666666666666</v>
       </c>
       <c r="R7">
         <v>19</v>
@@ -1123,12 +1109,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" t="s">
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D8">
         <v>160</v>
@@ -1137,10 +1123,10 @@
         <v>92</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G8">
-        <v>73.333333333333329</v>
+        <v>73.33333333333333</v>
       </c>
       <c r="H8">
         <v>44</v>
@@ -1155,7 +1141,7 @@
         <v>54</v>
       </c>
       <c r="L8">
-        <v>71.428571428571431</v>
+        <v>71.42857142857143</v>
       </c>
       <c r="M8">
         <v>15</v>
@@ -1170,7 +1156,7 @@
         <v>64</v>
       </c>
       <c r="Q8">
-        <v>80.952380952380949</v>
+        <v>80.95238095238095</v>
       </c>
       <c r="R8">
         <v>17</v>
@@ -1185,7 +1171,7 @@
         <v>42</v>
       </c>
       <c r="V8">
-        <v>66.666666666666657</v>
+        <v>66.66666666666666</v>
       </c>
       <c r="W8">
         <v>12</v>
@@ -1197,12 +1183,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25">
       <c r="B9" t="s">
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D9">
         <v>141</v>
@@ -1211,10 +1197,10 @@
         <v>88</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G9">
-        <v>67.796610169491515</v>
+        <v>67.79661016949152</v>
       </c>
       <c r="H9">
         <v>40</v>
@@ -1229,7 +1215,7 @@
         <v>57</v>
       </c>
       <c r="L9">
-        <v>69.565217391304344</v>
+        <v>69.56521739130434</v>
       </c>
       <c r="M9">
         <v>16</v>
@@ -1271,12 +1257,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25">
       <c r="B10" t="s">
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D10">
         <v>240</v>
@@ -1285,7 +1271,7 @@
         <v>99</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G10">
         <v>93.84615384615384</v>
@@ -1318,7 +1304,7 @@
         <v>77</v>
       </c>
       <c r="Q10">
-        <v>86.956521739130437</v>
+        <v>86.95652173913044</v>
       </c>
       <c r="R10">
         <v>20</v>
@@ -1345,12 +1331,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25">
       <c r="B11" t="s">
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D11">
         <v>246</v>
@@ -1359,7 +1345,7 @@
         <v>99</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G11">
         <v>96.875</v>
@@ -1419,12 +1405,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25">
       <c r="B12" t="s">
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D12">
         <v>225</v>
@@ -1433,7 +1419,7 @@
         <v>98</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G12">
         <v>95</v>
@@ -1451,7 +1437,7 @@
         <v>91</v>
       </c>
       <c r="L12">
-        <v>95.833333333333343</v>
+        <v>95.83333333333334</v>
       </c>
       <c r="M12">
         <v>23</v>
@@ -1466,7 +1452,7 @@
         <v>67</v>
       </c>
       <c r="Q12">
-        <v>94.444444444444443</v>
+        <v>94.44444444444444</v>
       </c>
       <c r="R12">
         <v>17</v>
@@ -1481,7 +1467,7 @@
         <v>67</v>
       </c>
       <c r="V12">
-        <v>94.444444444444443</v>
+        <v>94.44444444444444</v>
       </c>
       <c r="W12">
         <v>17</v>
@@ -1493,12 +1479,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="B13" t="s">
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D13">
         <v>227</v>
@@ -1507,10 +1493,10 @@
         <v>99</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G13">
-        <v>86.764705882352942</v>
+        <v>86.76470588235294</v>
       </c>
       <c r="H13">
         <v>59</v>
@@ -1525,7 +1511,7 @@
         <v>87</v>
       </c>
       <c r="L13">
-        <v>95.652173913043484</v>
+        <v>95.65217391304348</v>
       </c>
       <c r="M13">
         <v>22</v>
@@ -1540,7 +1526,7 @@
         <v>76</v>
       </c>
       <c r="Q13">
-        <v>83.333333333333343</v>
+        <v>83.33333333333334</v>
       </c>
       <c r="R13">
         <v>20</v>
@@ -1555,7 +1541,7 @@
         <v>64</v>
       </c>
       <c r="V13">
-        <v>80.952380952380949</v>
+        <v>80.95238095238095</v>
       </c>
       <c r="W13">
         <v>17</v>
@@ -1567,12 +1553,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="B14" t="s">
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D14">
         <v>229</v>
@@ -1581,10 +1567,10 @@
         <v>99</v>
       </c>
       <c r="F14" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G14">
-        <v>89.393939393939391</v>
+        <v>89.39393939393939</v>
       </c>
       <c r="H14">
         <v>59</v>
@@ -1599,7 +1585,7 @@
         <v>86</v>
       </c>
       <c r="L14">
-        <v>91.666666666666657</v>
+        <v>91.66666666666666</v>
       </c>
       <c r="M14">
         <v>22</v>
@@ -1614,7 +1600,7 @@
         <v>64</v>
       </c>
       <c r="Q14">
-        <v>80.952380952380949</v>
+        <v>80.95238095238095</v>
       </c>
       <c r="R14">
         <v>17</v>
@@ -1629,7 +1615,7 @@
         <v>79</v>
       </c>
       <c r="V14">
-        <v>95.238095238095227</v>
+        <v>95.23809523809523</v>
       </c>
       <c r="W14">
         <v>20</v>
@@ -1641,12 +1627,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="B15" t="s">
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D15">
         <v>213</v>
@@ -1655,10 +1641,10 @@
         <v>98</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G15">
-        <v>88.709677419354833</v>
+        <v>88.70967741935483</v>
       </c>
       <c r="H15">
         <v>55</v>
@@ -1673,7 +1659,7 @@
         <v>86</v>
       </c>
       <c r="L15">
-        <v>91.666666666666657</v>
+        <v>91.66666666666666</v>
       </c>
       <c r="M15">
         <v>22</v>
@@ -1688,7 +1674,7 @@
         <v>57</v>
       </c>
       <c r="Q15">
-        <v>83.333333333333343</v>
+        <v>83.33333333333334</v>
       </c>
       <c r="R15">
         <v>15</v>
@@ -1715,18 +1701,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="B16" t="s">
         <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D16">
         <v>208</v>
       </c>
       <c r="G16">
-        <v>82.089552238805979</v>
+        <v>82.08955223880598</v>
       </c>
       <c r="H16">
         <v>55</v>
@@ -1771,7 +1757,7 @@
         <v>53</v>
       </c>
       <c r="V16">
-        <v>68.181818181818173</v>
+        <v>68.18181818181817</v>
       </c>
       <c r="W16">
         <v>15</v>
@@ -1783,205 +1769,347 @@
         <v>3</v>
       </c>
     </row>
+    <row r="17" spans="2:25">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17">
+        <v>225</v>
+      </c>
+      <c r="G17">
+        <v>84.28571428571429</v>
+      </c>
+      <c r="H17">
+        <v>59</v>
+      </c>
+      <c r="I17">
+        <v>11</v>
+      </c>
+      <c r="J17">
+        <v>5</v>
+      </c>
+      <c r="K17">
+        <v>76</v>
+      </c>
+      <c r="L17">
+        <v>83.33333333333334</v>
+      </c>
+      <c r="M17">
+        <v>20</v>
+      </c>
+      <c r="N17">
+        <v>4</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>62</v>
+      </c>
+      <c r="Q17">
+        <v>73.91304347826086</v>
+      </c>
+      <c r="R17">
+        <v>17</v>
+      </c>
+      <c r="S17">
+        <v>6</v>
+      </c>
+      <c r="T17">
+        <v>2</v>
+      </c>
+      <c r="U17">
+        <v>87</v>
+      </c>
+      <c r="V17">
+        <v>95.65217391304348</v>
+      </c>
+      <c r="W17">
+        <v>22</v>
+      </c>
+      <c r="X17">
+        <v>1</v>
+      </c>
+      <c r="Y17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25">
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18">
+        <v>268</v>
+      </c>
+      <c r="E18">
+        <v>99</v>
+      </c>
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18">
+        <v>94.44444444444444</v>
+      </c>
+      <c r="H18">
+        <v>68</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>100</v>
+      </c>
+      <c r="L18">
+        <v>100</v>
+      </c>
+      <c r="M18">
+        <v>25</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>77</v>
+      </c>
+      <c r="Q18">
+        <v>86.95652173913044</v>
+      </c>
+      <c r="R18">
+        <v>20</v>
+      </c>
+      <c r="S18">
+        <v>3</v>
+      </c>
+      <c r="T18">
+        <v>2</v>
+      </c>
+      <c r="U18">
+        <v>91</v>
+      </c>
+      <c r="V18">
+        <v>95.83333333333334</v>
+      </c>
+      <c r="W18">
+        <v>23</v>
+      </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E16">
+  <conditionalFormatting sqref="E2:E18">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K16">
+  <conditionalFormatting sqref="K2:K18">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L16">
+  <conditionalFormatting sqref="L2:L18">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M16">
+  <conditionalFormatting sqref="M2:M18">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N16">
+  <conditionalFormatting sqref="N2:N18">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P16">
+  <conditionalFormatting sqref="P2:P18">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q16">
+  <conditionalFormatting sqref="Q2:Q18">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R16">
+  <conditionalFormatting sqref="R2:R18">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S16">
+  <conditionalFormatting sqref="S2:S18">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U16">
+  <conditionalFormatting sqref="U2:U18">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V16">
+  <conditionalFormatting sqref="V2:V18">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W16">
+  <conditionalFormatting sqref="W2:W18">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X16">
+  <conditionalFormatting sqref="X2:X18">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>

</xml_diff>

<commit_message>
9 Jan 2025 with Fix2
</commit_message>
<xml_diff>
--- a/Allen_Dark_Analysis.xlsx
+++ b/Allen_Dark_Analysis.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\CompSciFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C419D145-AFCF-4E3A-A222-774737995872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B387B40-A68C-49DC-9518-C24FC12FBCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
   <si>
     <t>Date</t>
   </si>
@@ -190,6 +203,36 @@
     <t>test28.mhtml</t>
   </si>
   <si>
+    <t>test29.mht</t>
+  </si>
+  <si>
+    <t>test30.mht</t>
+  </si>
+  <si>
+    <t>test31.mht</t>
+  </si>
+  <si>
+    <t>test32.mht</t>
+  </si>
+  <si>
+    <t>test33.mht</t>
+  </si>
+  <si>
+    <t>test34.mht</t>
+  </si>
+  <si>
+    <t>test35.mht</t>
+  </si>
+  <si>
+    <t>test36.mht</t>
+  </si>
+  <si>
+    <t>test37.mht</t>
+  </si>
+  <si>
+    <t>test38.mht</t>
+  </si>
+  <si>
     <t>JEE MAINS 24 Jan Shift 1 | 27th Dec,2024 | Online Mode</t>
   </si>
   <si>
@@ -283,6 +326,36 @@
     <t>JEE MAINS 03 April Shift 2 | 1st Jan,1 | Online Mode</t>
   </si>
   <si>
+    <t>JEE MAINS 29 Jan Shift 1 | 1st Jan,1 | Online Mode</t>
+  </si>
+  <si>
+    <t>JEE MAINS 29 Jan Shift 2 | 1st Jan,1 | Online Mode</t>
+  </si>
+  <si>
+    <t>JEE MAINS 07 April Shift 1 | 1st Jan,1 | Online Mode</t>
+  </si>
+  <si>
+    <t>JEE MAINS 07 April Shift 2 | 1st Jan,1 | Online Mode</t>
+  </si>
+  <si>
+    <t>JEE MAINS 23 Jan Shift 1 | 1st Jan,1 | Online Mode</t>
+  </si>
+  <si>
+    <t>JEE MAINS 23 Jan Shift 2 | 1st Jan,1 | Online Mode</t>
+  </si>
+  <si>
+    <t>JEE MAINS 22 Jan Shift 1 | 1st Jan,1 | Online Mode</t>
+  </si>
+  <si>
+    <t>JEE MAINS 22 Jan Shift 2 | 1st Jan,1 | Online Mode</t>
+  </si>
+  <si>
+    <t>JEE MAINS 02 April Shift 1 | 1st Jan,1 | Online Mode</t>
+  </si>
+  <si>
+    <t>JEE MAINS 02 April Shift 2 | 1st Jan,1 | Online Mode</t>
+  </si>
+  <si>
     <t>6015 to 6181</t>
   </si>
   <si>
@@ -359,6 +432,21 @@
   </si>
   <si>
     <t>614 to 655</t>
+  </si>
+  <si>
+    <t>17426 to 17840</t>
+  </si>
+  <si>
+    <t>6182 to 6348</t>
+  </si>
+  <si>
+    <t>3249 to 3391</t>
+  </si>
+  <si>
+    <t>2380 to 2467</t>
+  </si>
+  <si>
+    <t>434 to 457</t>
   </si>
 </sst>
 </file>
@@ -700,16 +788,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y32"/>
+  <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD42"/>
+    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
+      <selection activeCell="X41" sqref="X41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="3" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
@@ -805,7 +894,7 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D2">
         <v>193</v>
@@ -814,7 +903,7 @@
         <v>96</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="G2">
         <v>77.611940298507463</v>
@@ -829,9 +918,11 @@
         <v>8</v>
       </c>
       <c r="K2">
+        <f t="shared" ref="K2:K34" si="0">M2*4-N2</f>
         <v>67</v>
       </c>
       <c r="L2">
+        <f t="shared" ref="L2:M34" si="1">M2/(M2+N2)*100</f>
         <v>78.260869565217391</v>
       </c>
       <c r="M2">
@@ -841,12 +932,15 @@
         <v>5</v>
       </c>
       <c r="O2">
+        <f t="shared" ref="O2:O41" si="2">25-M2-N2</f>
         <v>2</v>
       </c>
       <c r="P2">
+        <f t="shared" ref="P2:P41" si="3">R2*4-S2</f>
         <v>63</v>
       </c>
       <c r="Q2">
+        <f t="shared" ref="Q2:Q42" si="4">R2/(R2+S2)*100</f>
         <v>77.272727272727266</v>
       </c>
       <c r="R2">
@@ -856,12 +950,15 @@
         <v>5</v>
       </c>
       <c r="T2">
+        <f t="shared" ref="T2:T41" si="5">25-R2-S2</f>
         <v>3</v>
       </c>
       <c r="U2">
+        <f t="shared" ref="U2:U41" si="6">W2*4-X2</f>
         <v>63</v>
       </c>
       <c r="V2">
+        <f t="shared" ref="V2:V41" si="7">W2/(W2+X2)*100</f>
         <v>77.272727272727266</v>
       </c>
       <c r="W2">
@@ -871,6 +968,7 @@
         <v>5</v>
       </c>
       <c r="Y2">
+        <f t="shared" ref="Y2:Y37" si="8">25-W2-X2</f>
         <v>3</v>
       </c>
     </row>
@@ -879,7 +977,7 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D3">
         <v>178</v>
@@ -888,7 +986,7 @@
         <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="G3">
         <v>77.41935483870968</v>
@@ -903,9 +1001,11 @@
         <v>13</v>
       </c>
       <c r="K3">
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="L3">
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="M3">
@@ -915,12 +1015,15 @@
         <v>2</v>
       </c>
       <c r="O3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P3">
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="Q3">
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="R3">
@@ -930,12 +1033,15 @@
         <v>8</v>
       </c>
       <c r="T3">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="U3">
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="V3">
+        <f t="shared" si="7"/>
         <v>76.470588235294116</v>
       </c>
       <c r="W3">
@@ -945,6 +1051,7 @@
         <v>4</v>
       </c>
       <c r="Y3">
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
     </row>
@@ -953,7 +1060,7 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D4">
         <v>155</v>
@@ -962,7 +1069,7 @@
         <v>91</v>
       </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="G4">
         <v>71.666666666666671</v>
@@ -977,9 +1084,11 @@
         <v>15</v>
       </c>
       <c r="K4">
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="L4">
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="M4">
@@ -989,13 +1098,16 @@
         <v>2</v>
       </c>
       <c r="O4">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="P4">
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="Q4">
-        <v>61.904761904761912</v>
+        <f t="shared" si="4"/>
+        <v>61.904761904761905</v>
       </c>
       <c r="R4">
         <v>13</v>
@@ -1004,12 +1116,15 @@
         <v>8</v>
       </c>
       <c r="T4">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="U4">
+        <f t="shared" si="6"/>
         <v>41</v>
       </c>
       <c r="V4">
+        <f t="shared" si="7"/>
         <v>63.157894736842103</v>
       </c>
       <c r="W4">
@@ -1019,6 +1134,7 @@
         <v>7</v>
       </c>
       <c r="Y4">
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
     </row>
@@ -1027,7 +1143,7 @@
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D5">
         <v>164</v>
@@ -1036,7 +1152,7 @@
         <v>93</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="G5">
         <v>69.696969696969703</v>
@@ -1051,9 +1167,11 @@
         <v>9</v>
       </c>
       <c r="K5">
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="L5">
+        <f t="shared" si="1"/>
         <v>79.166666666666657</v>
       </c>
       <c r="M5">
@@ -1063,12 +1181,15 @@
         <v>5</v>
       </c>
       <c r="O5">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P5">
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="Q5">
+        <f t="shared" si="4"/>
         <v>59.090909090909093</v>
       </c>
       <c r="R5">
@@ -1078,12 +1199,15 @@
         <v>9</v>
       </c>
       <c r="T5">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="U5">
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="V5">
+        <f t="shared" si="7"/>
         <v>70</v>
       </c>
       <c r="W5">
@@ -1093,6 +1217,7 @@
         <v>6</v>
       </c>
       <c r="Y5">
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
     </row>
@@ -1101,7 +1226,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>222</v>
@@ -1110,7 +1235,7 @@
         <v>98</v>
       </c>
       <c r="F6" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="G6">
         <v>85.294117647058826</v>
@@ -1125,9 +1250,11 @@
         <v>7</v>
       </c>
       <c r="K6">
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="L6">
+        <f t="shared" si="1"/>
         <v>73.91304347826086</v>
       </c>
       <c r="M6">
@@ -1137,12 +1264,15 @@
         <v>6</v>
       </c>
       <c r="O6">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="P6">
+        <f t="shared" si="3"/>
         <v>78</v>
       </c>
       <c r="Q6">
+        <f t="shared" si="4"/>
         <v>90.909090909090907</v>
       </c>
       <c r="R6">
@@ -1152,12 +1282,15 @@
         <v>2</v>
       </c>
       <c r="T6">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="U6">
+        <f t="shared" si="6"/>
         <v>82</v>
       </c>
       <c r="V6">
+        <f t="shared" si="7"/>
         <v>91.304347826086953</v>
       </c>
       <c r="W6">
@@ -1167,6 +1300,7 @@
         <v>2</v>
       </c>
       <c r="Y6">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -1175,7 +1309,7 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D7">
         <v>210</v>
@@ -1184,7 +1318,7 @@
         <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="G7">
         <v>84.615384615384613</v>
@@ -1199,9 +1333,11 @@
         <v>10</v>
       </c>
       <c r="K7">
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="L7">
+        <f t="shared" si="1"/>
         <v>79.166666666666657</v>
       </c>
       <c r="M7">
@@ -1211,12 +1347,15 @@
         <v>5</v>
       </c>
       <c r="O7">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P7">
+        <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="Q7">
+        <f t="shared" si="4"/>
         <v>79.166666666666657</v>
       </c>
       <c r="R7">
@@ -1226,12 +1365,15 @@
         <v>5</v>
       </c>
       <c r="T7">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U7">
+        <f t="shared" si="6"/>
         <v>68</v>
       </c>
       <c r="V7">
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="W7">
@@ -1241,6 +1383,7 @@
         <v>0</v>
       </c>
       <c r="Y7">
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
     </row>
@@ -1249,7 +1392,7 @@
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="D8">
         <v>160</v>
@@ -1258,7 +1401,7 @@
         <v>92</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="G8">
         <v>73.333333333333329</v>
@@ -1273,9 +1416,11 @@
         <v>15</v>
       </c>
       <c r="K8">
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="L8">
+        <f t="shared" si="1"/>
         <v>71.428571428571431</v>
       </c>
       <c r="M8">
@@ -1285,12 +1430,15 @@
         <v>6</v>
       </c>
       <c r="O8">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="P8">
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="Q8">
+        <f>R8/(R8+S8)*100</f>
         <v>80.952380952380949</v>
       </c>
       <c r="R8">
@@ -1300,12 +1448,15 @@
         <v>4</v>
       </c>
       <c r="T8">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="U8">
+        <f t="shared" si="6"/>
         <v>42</v>
       </c>
       <c r="V8">
+        <f t="shared" si="7"/>
         <v>66.666666666666657</v>
       </c>
       <c r="W8">
@@ -1315,6 +1466,7 @@
         <v>6</v>
       </c>
       <c r="Y8">
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
     </row>
@@ -1323,7 +1475,7 @@
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D9">
         <v>141</v>
@@ -1332,7 +1484,7 @@
         <v>88</v>
       </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="G9">
         <v>67.796610169491515</v>
@@ -1347,9 +1499,11 @@
         <v>16</v>
       </c>
       <c r="K9">
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="L9">
+        <f t="shared" si="1"/>
         <v>69.565217391304344</v>
       </c>
       <c r="M9">
@@ -1359,12 +1513,15 @@
         <v>7</v>
       </c>
       <c r="O9">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="P9">
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="Q9">
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="R9">
@@ -1374,12 +1531,15 @@
         <v>7</v>
       </c>
       <c r="T9">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="U9">
+        <f t="shared" si="6"/>
         <v>39</v>
       </c>
       <c r="V9">
+        <f t="shared" si="7"/>
         <v>68.75</v>
       </c>
       <c r="W9">
@@ -1389,6 +1549,7 @@
         <v>5</v>
       </c>
       <c r="Y9">
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
     </row>
@@ -1397,7 +1558,7 @@
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="D10">
         <v>240</v>
@@ -1406,7 +1567,7 @@
         <v>99</v>
       </c>
       <c r="F10" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="G10">
         <v>93.84615384615384</v>
@@ -1421,9 +1582,11 @@
         <v>10</v>
       </c>
       <c r="K10">
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="L10">
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
       <c r="M10">
@@ -1433,12 +1596,15 @@
         <v>1</v>
       </c>
       <c r="O10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P10">
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="Q10">
+        <f t="shared" si="4"/>
         <v>86.956521739130437</v>
       </c>
       <c r="R10">
@@ -1448,12 +1614,15 @@
         <v>3</v>
       </c>
       <c r="T10">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="U10">
+        <f t="shared" si="6"/>
         <v>68</v>
       </c>
       <c r="V10">
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="W10">
@@ -1463,6 +1632,7 @@
         <v>0</v>
       </c>
       <c r="Y10">
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
     </row>
@@ -1471,7 +1641,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D11">
         <v>246</v>
@@ -1480,7 +1650,7 @@
         <v>99</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="G11">
         <v>96.875</v>
@@ -1495,9 +1665,11 @@
         <v>11</v>
       </c>
       <c r="K11">
+        <f t="shared" si="0"/>
         <v>96</v>
       </c>
       <c r="L11">
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="M11">
@@ -1507,12 +1679,15 @@
         <v>0</v>
       </c>
       <c r="O11">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P11">
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="Q11">
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="R11">
@@ -1522,12 +1697,15 @@
         <v>0</v>
       </c>
       <c r="T11">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U11">
+        <f t="shared" si="6"/>
         <v>54</v>
       </c>
       <c r="V11">
+        <f t="shared" si="7"/>
         <v>87.5</v>
       </c>
       <c r="W11">
@@ -1537,6 +1715,7 @@
         <v>2</v>
       </c>
       <c r="Y11">
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
     </row>
@@ -1545,7 +1724,7 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D12">
         <v>225</v>
@@ -1554,7 +1733,7 @@
         <v>98</v>
       </c>
       <c r="F12" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="G12">
         <v>95</v>
@@ -1569,9 +1748,11 @@
         <v>15</v>
       </c>
       <c r="K12">
+        <f t="shared" si="0"/>
         <v>91</v>
       </c>
       <c r="L12">
+        <f t="shared" si="1"/>
         <v>95.833333333333343</v>
       </c>
       <c r="M12">
@@ -1581,12 +1762,15 @@
         <v>1</v>
       </c>
       <c r="O12">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P12">
+        <f t="shared" si="3"/>
         <v>67</v>
       </c>
       <c r="Q12">
+        <f t="shared" si="4"/>
         <v>94.444444444444443</v>
       </c>
       <c r="R12">
@@ -1596,12 +1780,15 @@
         <v>1</v>
       </c>
       <c r="T12">
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="U12">
+        <f t="shared" si="6"/>
         <v>67</v>
       </c>
       <c r="V12">
+        <f t="shared" si="7"/>
         <v>94.444444444444443</v>
       </c>
       <c r="W12">
@@ -1611,6 +1798,7 @@
         <v>1</v>
       </c>
       <c r="Y12">
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
     </row>
@@ -1619,7 +1807,7 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D13">
         <v>227</v>
@@ -1628,7 +1816,7 @@
         <v>99</v>
       </c>
       <c r="F13" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="G13">
         <v>86.764705882352942</v>
@@ -1643,9 +1831,11 @@
         <v>7</v>
       </c>
       <c r="K13">
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
       <c r="L13">
+        <f t="shared" si="1"/>
         <v>95.652173913043484</v>
       </c>
       <c r="M13">
@@ -1655,12 +1845,15 @@
         <v>1</v>
       </c>
       <c r="O13">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="P13">
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
       <c r="Q13">
+        <f t="shared" si="4"/>
         <v>83.333333333333343</v>
       </c>
       <c r="R13">
@@ -1670,12 +1863,15 @@
         <v>4</v>
       </c>
       <c r="T13">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U13">
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="V13">
+        <f t="shared" si="7"/>
         <v>80.952380952380949</v>
       </c>
       <c r="W13">
@@ -1685,6 +1881,7 @@
         <v>4</v>
       </c>
       <c r="Y13">
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
     </row>
@@ -1693,7 +1890,7 @@
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D14">
         <v>229</v>
@@ -1702,7 +1899,7 @@
         <v>99</v>
       </c>
       <c r="F14" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="G14">
         <v>89.393939393939391</v>
@@ -1717,9 +1914,11 @@
         <v>9</v>
       </c>
       <c r="K14">
+        <f t="shared" si="0"/>
         <v>86</v>
       </c>
       <c r="L14">
+        <f t="shared" si="1"/>
         <v>91.666666666666657</v>
       </c>
       <c r="M14">
@@ -1729,12 +1928,15 @@
         <v>2</v>
       </c>
       <c r="O14">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P14">
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="Q14">
+        <f t="shared" si="4"/>
         <v>80.952380952380949</v>
       </c>
       <c r="R14">
@@ -1744,12 +1946,15 @@
         <v>4</v>
       </c>
       <c r="T14">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="U14">
+        <f t="shared" si="6"/>
         <v>79</v>
       </c>
       <c r="V14">
+        <f t="shared" si="7"/>
         <v>95.238095238095227</v>
       </c>
       <c r="W14">
@@ -1759,6 +1964,7 @@
         <v>1</v>
       </c>
       <c r="Y14">
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
     </row>
@@ -1767,7 +1973,7 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="D15">
         <v>213</v>
@@ -1776,7 +1982,7 @@
         <v>98</v>
       </c>
       <c r="F15" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G15">
         <v>88.709677419354833</v>
@@ -1791,9 +1997,11 @@
         <v>13</v>
       </c>
       <c r="K15">
+        <f t="shared" si="0"/>
         <v>86</v>
       </c>
       <c r="L15">
+        <f t="shared" si="1"/>
         <v>91.666666666666657</v>
       </c>
       <c r="M15">
@@ -1803,12 +2011,15 @@
         <v>2</v>
       </c>
       <c r="O15">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P15">
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="Q15">
+        <f t="shared" si="4"/>
         <v>83.333333333333343</v>
       </c>
       <c r="R15">
@@ -1818,12 +2029,15 @@
         <v>3</v>
       </c>
       <c r="T15">
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="U15">
+        <f t="shared" si="6"/>
         <v>70</v>
       </c>
       <c r="V15">
+        <f t="shared" si="7"/>
         <v>90</v>
       </c>
       <c r="W15">
@@ -1833,6 +2047,7 @@
         <v>2</v>
       </c>
       <c r="Y15">
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
     </row>
@@ -1841,7 +2056,7 @@
         <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D16">
         <v>208</v>
@@ -1859,9 +2074,11 @@
         <v>23</v>
       </c>
       <c r="K16">
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="L16">
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
       <c r="M16">
@@ -1871,12 +2088,15 @@
         <v>1</v>
       </c>
       <c r="O16">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P16">
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="Q16">
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="R16">
@@ -1886,12 +2106,15 @@
         <v>4</v>
       </c>
       <c r="T16">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="U16">
+        <f t="shared" si="6"/>
         <v>53</v>
       </c>
       <c r="V16">
+        <f t="shared" si="7"/>
         <v>68.181818181818173</v>
       </c>
       <c r="W16">
@@ -1901,6 +2124,7 @@
         <v>7</v>
       </c>
       <c r="Y16">
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
     </row>
@@ -1909,7 +2133,7 @@
         <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D17">
         <v>225</v>
@@ -1927,9 +2151,11 @@
         <v>5</v>
       </c>
       <c r="K17">
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="L17">
+        <f t="shared" si="1"/>
         <v>83.333333333333343</v>
       </c>
       <c r="M17">
@@ -1939,12 +2165,15 @@
         <v>4</v>
       </c>
       <c r="O17">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P17">
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
       <c r="Q17">
+        <f t="shared" si="4"/>
         <v>73.91304347826086</v>
       </c>
       <c r="R17">
@@ -1954,12 +2183,15 @@
         <v>6</v>
       </c>
       <c r="T17">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="U17">
+        <f t="shared" si="6"/>
         <v>87</v>
       </c>
       <c r="V17">
+        <f t="shared" si="7"/>
         <v>95.652173913043484</v>
       </c>
       <c r="W17">
@@ -1969,6 +2201,7 @@
         <v>1</v>
       </c>
       <c r="Y17">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -1977,7 +2210,7 @@
         <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D18">
         <v>268</v>
@@ -1986,7 +2219,7 @@
         <v>99</v>
       </c>
       <c r="F18" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="G18">
         <v>94.444444444444443</v>
@@ -2001,9 +2234,11 @@
         <v>3</v>
       </c>
       <c r="K18">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="L18">
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="M18">
@@ -2013,12 +2248,15 @@
         <v>0</v>
       </c>
       <c r="O18">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P18">
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="Q18">
+        <f t="shared" si="4"/>
         <v>86.956521739130437</v>
       </c>
       <c r="R18">
@@ -2028,12 +2266,15 @@
         <v>3</v>
       </c>
       <c r="T18">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="U18">
+        <f t="shared" si="6"/>
         <v>91</v>
       </c>
       <c r="V18">
+        <f t="shared" si="7"/>
         <v>95.833333333333343</v>
       </c>
       <c r="W18">
@@ -2043,6 +2284,7 @@
         <v>1</v>
       </c>
       <c r="Y18">
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -2051,7 +2293,7 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="D19">
         <v>226</v>
@@ -2060,7 +2302,7 @@
         <v>98</v>
       </c>
       <c r="F19" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="G19">
         <v>85.507246376811594</v>
@@ -2075,9 +2317,11 @@
         <v>6</v>
       </c>
       <c r="K19">
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="L19">
+        <f t="shared" si="1"/>
         <v>78.260869565217391</v>
       </c>
       <c r="M19">
@@ -2087,12 +2331,15 @@
         <v>5</v>
       </c>
       <c r="O19">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="P19">
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
       <c r="Q19">
+        <f t="shared" si="4"/>
         <v>91.666666666666657</v>
       </c>
       <c r="R19">
@@ -2102,12 +2349,15 @@
         <v>2</v>
       </c>
       <c r="T19">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U19">
+        <f t="shared" si="6"/>
         <v>73</v>
       </c>
       <c r="V19">
+        <f t="shared" si="7"/>
         <v>86.36363636363636</v>
       </c>
       <c r="W19">
@@ -2117,6 +2367,7 @@
         <v>3</v>
       </c>
       <c r="Y19">
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
     </row>
@@ -2125,7 +2376,7 @@
         <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D20">
         <v>225</v>
@@ -2134,7 +2385,7 @@
         <v>98</v>
       </c>
       <c r="F20" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="G20">
         <v>84.285714285714292</v>
@@ -2149,9 +2400,11 @@
         <v>5</v>
       </c>
       <c r="K20">
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="L20">
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="M20">
@@ -2161,12 +2414,15 @@
         <v>5</v>
       </c>
       <c r="O20">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P20">
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="Q20">
+        <f t="shared" si="4"/>
         <v>86.956521739130437</v>
       </c>
       <c r="R20">
@@ -2176,12 +2432,15 @@
         <v>3</v>
       </c>
       <c r="T20">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="U20">
+        <f t="shared" si="6"/>
         <v>73</v>
       </c>
       <c r="V20">
+        <f t="shared" si="7"/>
         <v>86.36363636363636</v>
       </c>
       <c r="W20">
@@ -2191,6 +2450,7 @@
         <v>3</v>
       </c>
       <c r="Y20">
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
     </row>
@@ -2199,7 +2459,7 @@
         <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D21">
         <v>194</v>
@@ -2208,7 +2468,7 @@
         <v>97</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="G21">
         <v>78.787878787878782</v>
@@ -2223,9 +2483,11 @@
         <v>9</v>
       </c>
       <c r="K21">
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="L21">
+        <f t="shared" si="1"/>
         <v>79.166666666666657</v>
       </c>
       <c r="M21">
@@ -2235,12 +2497,15 @@
         <v>5</v>
       </c>
       <c r="O21">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P21">
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="Q21">
+        <f t="shared" si="4"/>
         <v>68.421052631578945</v>
       </c>
       <c r="R21">
@@ -2250,12 +2515,15 @@
         <v>6</v>
       </c>
       <c r="T21">
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="U21">
+        <f t="shared" si="6"/>
         <v>77</v>
       </c>
       <c r="V21">
+        <f t="shared" si="7"/>
         <v>86.956521739130437</v>
       </c>
       <c r="W21">
@@ -2265,6 +2533,7 @@
         <v>3</v>
       </c>
       <c r="Y21">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2273,7 +2542,7 @@
         <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D22">
         <v>217</v>
@@ -2282,7 +2551,7 @@
         <v>98</v>
       </c>
       <c r="F22" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="G22">
         <v>83.82352941176471</v>
@@ -2297,9 +2566,11 @@
         <v>7</v>
       </c>
       <c r="K22">
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="L22">
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="M22">
@@ -2309,12 +2580,15 @@
         <v>2</v>
       </c>
       <c r="O22">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P22">
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="Q22">
+        <f t="shared" si="4"/>
         <v>52.631578947368418</v>
       </c>
       <c r="R22">
@@ -2324,12 +2598,15 @@
         <v>9</v>
       </c>
       <c r="T22">
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="U22">
+        <f t="shared" si="6"/>
         <v>96</v>
       </c>
       <c r="V22">
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="W22">
@@ -2339,6 +2616,7 @@
         <v>0</v>
       </c>
       <c r="Y22">
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -2347,7 +2625,7 @@
         <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="D23">
         <v>233</v>
@@ -2356,7 +2634,7 @@
         <v>99</v>
       </c>
       <c r="F23" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="G23">
         <v>95.161290322580655</v>
@@ -2371,9 +2649,11 @@
         <v>13</v>
       </c>
       <c r="K23">
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="L23">
+        <f t="shared" si="1"/>
         <v>86.956521739130437</v>
       </c>
       <c r="M23">
@@ -2383,12 +2663,15 @@
         <v>3</v>
       </c>
       <c r="O23">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="P23">
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
       <c r="Q23">
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="R23">
@@ -2398,12 +2681,15 @@
         <v>0</v>
       </c>
       <c r="T23">
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="U23">
+        <f t="shared" si="6"/>
         <v>80</v>
       </c>
       <c r="V23">
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="W23">
@@ -2413,6 +2699,7 @@
         <v>0</v>
       </c>
       <c r="Y23">
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
     </row>
@@ -2421,7 +2708,7 @@
         <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="D24">
         <v>230</v>
@@ -2430,7 +2717,7 @@
         <v>99</v>
       </c>
       <c r="F24" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="G24">
         <v>90.769230769230774</v>
@@ -2445,9 +2732,11 @@
         <v>10</v>
       </c>
       <c r="K24">
+        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="L24">
+        <f t="shared" si="1"/>
         <v>90.476190476190482</v>
       </c>
       <c r="M24">
@@ -2457,12 +2746,15 @@
         <v>2</v>
       </c>
       <c r="O24">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="P24">
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
       <c r="Q24">
+        <f t="shared" si="4"/>
         <v>95.833333333333343</v>
       </c>
       <c r="R24">
@@ -2472,12 +2764,15 @@
         <v>1</v>
       </c>
       <c r="T24">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U24">
+        <f t="shared" si="6"/>
         <v>65</v>
       </c>
       <c r="V24">
+        <f t="shared" si="7"/>
         <v>85</v>
       </c>
       <c r="W24">
@@ -2487,6 +2782,7 @@
         <v>3</v>
       </c>
       <c r="Y24">
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
     </row>
@@ -2495,7 +2791,7 @@
         <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D25">
         <v>206</v>
@@ -2504,7 +2800,7 @@
         <v>98</v>
       </c>
       <c r="F25" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="G25">
         <v>84.375</v>
@@ -2519,9 +2815,11 @@
         <v>11</v>
       </c>
       <c r="K25">
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="L25">
+        <f t="shared" si="1"/>
         <v>87.5</v>
       </c>
       <c r="M25">
@@ -2531,12 +2829,15 @@
         <v>3</v>
       </c>
       <c r="O25">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P25">
+        <f t="shared" si="3"/>
         <v>59</v>
       </c>
       <c r="Q25">
+        <f t="shared" si="4"/>
         <v>76.19047619047619</v>
       </c>
       <c r="R25">
@@ -2546,12 +2847,15 @@
         <v>5</v>
       </c>
       <c r="T25">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="U25">
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
       <c r="V25">
+        <f t="shared" si="7"/>
         <v>89.473684210526315</v>
       </c>
       <c r="W25">
@@ -2561,6 +2865,7 @@
         <v>2</v>
       </c>
       <c r="Y25">
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
     </row>
@@ -2569,7 +2874,7 @@
         <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D26">
         <v>205</v>
@@ -2578,7 +2883,7 @@
         <v>98</v>
       </c>
       <c r="F26" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="G26">
         <v>78.571428571428569</v>
@@ -2593,9 +2898,11 @@
         <v>5</v>
       </c>
       <c r="K26">
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="L26">
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="M26">
@@ -2605,12 +2912,15 @@
         <v>6</v>
       </c>
       <c r="O26">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P26">
+        <f t="shared" si="3"/>
         <v>68</v>
       </c>
       <c r="Q26">
+        <f t="shared" si="4"/>
         <v>81.818181818181827</v>
       </c>
       <c r="R26">
@@ -2620,12 +2930,15 @@
         <v>4</v>
       </c>
       <c r="T26">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="U26">
+        <f t="shared" si="6"/>
         <v>71</v>
       </c>
       <c r="V26">
+        <f t="shared" si="7"/>
         <v>79.166666666666657</v>
       </c>
       <c r="W26">
@@ -2635,6 +2948,7 @@
         <v>5</v>
       </c>
       <c r="Y26">
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -2643,7 +2957,7 @@
         <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="D27">
         <v>159</v>
@@ -2652,7 +2966,7 @@
         <v>92</v>
       </c>
       <c r="F27" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="G27">
         <v>82.35294117647058</v>
@@ -2667,9 +2981,11 @@
         <v>24</v>
       </c>
       <c r="K27">
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="L27">
+        <f t="shared" si="1"/>
         <v>76.19047619047619</v>
       </c>
       <c r="M27">
@@ -2679,12 +2995,15 @@
         <v>5</v>
       </c>
       <c r="O27">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="P27">
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="Q27">
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="R27">
@@ -2694,12 +3013,15 @@
         <v>4</v>
       </c>
       <c r="T27">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="U27">
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="V27">
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="W27">
@@ -2709,6 +3031,7 @@
         <v>0</v>
       </c>
       <c r="Y27">
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
     </row>
@@ -2717,7 +3040,7 @@
         <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D28">
         <v>187</v>
@@ -2726,7 +3049,7 @@
         <v>96</v>
       </c>
       <c r="F28" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="G28">
         <v>79.365079365079367</v>
@@ -2741,9 +3064,11 @@
         <v>12</v>
       </c>
       <c r="K28">
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="L28">
+        <f t="shared" si="1"/>
         <v>83.333333333333343</v>
       </c>
       <c r="M28">
@@ -2753,12 +3078,15 @@
         <v>4</v>
       </c>
       <c r="O28">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P28">
+        <f t="shared" si="3"/>
         <v>68</v>
       </c>
       <c r="Q28">
+        <f t="shared" si="4"/>
         <v>81.818181818181827</v>
       </c>
       <c r="R28">
@@ -2768,12 +3096,15 @@
         <v>4</v>
       </c>
       <c r="T28">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="U28">
+        <f t="shared" si="6"/>
         <v>43</v>
       </c>
       <c r="V28">
+        <f t="shared" si="7"/>
         <v>70.588235294117652</v>
       </c>
       <c r="W28">
@@ -2783,6 +3114,7 @@
         <v>5</v>
       </c>
       <c r="Y28">
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
     </row>
@@ -2791,7 +3123,7 @@
         <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D29">
         <v>153</v>
@@ -2800,7 +3132,7 @@
         <v>91</v>
       </c>
       <c r="F29" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="G29">
         <v>73.68421052631578</v>
@@ -2815,9 +3147,11 @@
         <v>18</v>
       </c>
       <c r="K29">
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="L29">
+        <f t="shared" si="1"/>
         <v>73.91304347826086</v>
       </c>
       <c r="M29">
@@ -2827,12 +3161,15 @@
         <v>6</v>
       </c>
       <c r="O29">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="P29">
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="Q29">
+        <f t="shared" si="4"/>
         <v>76.470588235294116</v>
       </c>
       <c r="R29">
@@ -2842,12 +3179,15 @@
         <v>4</v>
       </c>
       <c r="T29">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="U29">
+        <f t="shared" si="6"/>
         <v>43</v>
       </c>
       <c r="V29">
+        <f t="shared" si="7"/>
         <v>70.588235294117652</v>
       </c>
       <c r="W29">
@@ -2857,6 +3197,7 @@
         <v>5</v>
       </c>
       <c r="Y29">
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
     </row>
@@ -2865,7 +3206,7 @@
         <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="D30">
         <v>249</v>
@@ -2874,7 +3215,7 @@
         <v>99</v>
       </c>
       <c r="F30" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="G30">
         <v>90.140845070422543</v>
@@ -2889,9 +3230,11 @@
         <v>4</v>
       </c>
       <c r="K30">
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="L30">
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="M30">
@@ -2901,12 +3244,15 @@
         <v>2</v>
       </c>
       <c r="O30">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P30">
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
       <c r="Q30">
+        <f t="shared" si="4"/>
         <v>77.272727272727266</v>
       </c>
       <c r="R30">
@@ -2916,12 +3262,15 @@
         <v>5</v>
       </c>
       <c r="T30">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="U30">
+        <f t="shared" si="6"/>
         <v>96</v>
       </c>
       <c r="V30">
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="W30">
@@ -2931,6 +3280,7 @@
         <v>0</v>
       </c>
       <c r="Y30">
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -2939,7 +3289,7 @@
         <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D31">
         <v>171</v>
@@ -2957,9 +3307,11 @@
         <v>6</v>
       </c>
       <c r="K31">
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="L31">
+        <f t="shared" si="1"/>
         <v>60.869565217391312</v>
       </c>
       <c r="M31">
@@ -2969,12 +3321,15 @@
         <v>9</v>
       </c>
       <c r="O31">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="P31">
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="Q31">
+        <f t="shared" si="4"/>
         <v>52.173913043478258</v>
       </c>
       <c r="R31">
@@ -2984,12 +3339,15 @@
         <v>11</v>
       </c>
       <c r="T31">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="U31">
+        <f t="shared" si="6"/>
         <v>87</v>
       </c>
       <c r="V31">
+        <f t="shared" si="7"/>
         <v>95.652173913043484</v>
       </c>
       <c r="W31">
@@ -2999,6 +3357,7 @@
         <v>1</v>
       </c>
       <c r="Y31">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -3007,7 +3366,7 @@
         <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="D32">
         <v>224</v>
@@ -3025,9 +3384,11 @@
         <v>4</v>
       </c>
       <c r="K32">
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="L32">
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="M32">
@@ -3037,12 +3398,15 @@
         <v>6</v>
       </c>
       <c r="O32">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P32">
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
       <c r="Q32">
+        <f t="shared" si="4"/>
         <v>72.727272727272734</v>
       </c>
       <c r="R32">
@@ -3052,12 +3416,15 @@
         <v>6</v>
       </c>
       <c r="T32">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="U32">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="V32">
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="W32">
@@ -3067,6 +3434,813 @@
         <v>0</v>
       </c>
       <c r="Y32">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33">
+        <v>157</v>
+      </c>
+      <c r="E33">
+        <v>91</v>
+      </c>
+      <c r="F33" t="s">
+        <v>133</v>
+      </c>
+      <c r="G33">
+        <v>74.137931034482762</v>
+      </c>
+      <c r="H33">
+        <v>43</v>
+      </c>
+      <c r="I33">
+        <v>15</v>
+      </c>
+      <c r="J33">
+        <v>17</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="M33">
+        <v>18</v>
+      </c>
+      <c r="N33">
+        <v>7</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="4"/>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="R33">
+        <v>15</v>
+      </c>
+      <c r="S33">
+        <v>3</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="7"/>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="W33">
+        <v>10</v>
+      </c>
+      <c r="X33">
+        <v>5</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34">
+        <v>192</v>
+      </c>
+      <c r="E34">
+        <v>96</v>
+      </c>
+      <c r="F34" t="s">
+        <v>134</v>
+      </c>
+      <c r="G34">
+        <v>76.470588235294116</v>
+      </c>
+      <c r="H34">
+        <v>52</v>
+      </c>
+      <c r="I34">
+        <v>16</v>
+      </c>
+      <c r="J34">
+        <v>7</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="1"/>
+        <v>62.5</v>
+      </c>
+      <c r="M34">
+        <v>15</v>
+      </c>
+      <c r="N34">
+        <v>9</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="4"/>
+        <v>68.181818181818173</v>
+      </c>
+      <c r="R34">
+        <v>15</v>
+      </c>
+      <c r="S34">
+        <v>7</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="6"/>
+        <v>88</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="W34">
+        <v>22</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35">
+        <v>220</v>
+      </c>
+      <c r="G35">
+        <v>82.857142857142861</v>
+      </c>
+      <c r="H35">
+        <v>58</v>
+      </c>
+      <c r="I35">
+        <v>12</v>
+      </c>
+      <c r="J35">
+        <v>5</v>
+      </c>
+      <c r="K35">
+        <f>M35*4-N35</f>
+        <v>91</v>
+      </c>
+      <c r="L35">
+        <f>M35/(M35+N35)*100</f>
+        <v>95.833333333333343</v>
+      </c>
+      <c r="M35">
+        <v>23</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="4"/>
+        <v>68.181818181818173</v>
+      </c>
+      <c r="R35">
+        <v>15</v>
+      </c>
+      <c r="S35">
+        <v>7</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="6"/>
+        <v>76</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="7"/>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="W35">
+        <v>20</v>
+      </c>
+      <c r="X35">
+        <v>4</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36">
+        <v>183</v>
+      </c>
+      <c r="G36">
+        <v>74.626865671641795</v>
+      </c>
+      <c r="H36">
+        <v>50</v>
+      </c>
+      <c r="I36">
+        <v>17</v>
+      </c>
+      <c r="J36">
+        <v>8</v>
+      </c>
+      <c r="K36">
+        <f t="shared" ref="K36:K42" si="9">M36*4-N36</f>
+        <v>68</v>
+      </c>
+      <c r="L36">
+        <f t="shared" ref="L36:M42" si="10">M36/(M36+N36)*100</f>
+        <v>81.818181818181827</v>
+      </c>
+      <c r="M36">
+        <v>18</v>
+      </c>
+      <c r="N36">
+        <v>4</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="4"/>
+        <v>54.54545454545454</v>
+      </c>
+      <c r="R36">
+        <v>12</v>
+      </c>
+      <c r="S36">
+        <v>10</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="6"/>
+        <v>78</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="7"/>
+        <v>90.909090909090907</v>
+      </c>
+      <c r="W36">
+        <v>20</v>
+      </c>
+      <c r="X36">
+        <v>2</v>
+      </c>
+      <c r="Y36">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37">
+        <v>211</v>
+      </c>
+      <c r="E37">
+        <v>98</v>
+      </c>
+      <c r="F37" t="s">
+        <v>135</v>
+      </c>
+      <c r="G37">
+        <v>81.159420289855078</v>
+      </c>
+      <c r="H37">
+        <v>56</v>
+      </c>
+      <c r="I37">
+        <v>13</v>
+      </c>
+      <c r="J37">
+        <v>6</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="9"/>
+        <v>80</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="10"/>
+        <v>84</v>
+      </c>
+      <c r="M37">
+        <v>21</v>
+      </c>
+      <c r="N37">
+        <v>4</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="4"/>
+        <v>90.476190476190482</v>
+      </c>
+      <c r="R37">
+        <v>19</v>
+      </c>
+      <c r="S37">
+        <v>2</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="6"/>
+        <v>57</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="7"/>
+        <v>69.565217391304344</v>
+      </c>
+      <c r="W37">
+        <v>16</v>
+      </c>
+      <c r="X37">
+        <v>7</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38">
+        <v>219</v>
+      </c>
+      <c r="E38">
+        <v>98</v>
+      </c>
+      <c r="F38" t="s">
+        <v>136</v>
+      </c>
+      <c r="G38">
+        <v>81.690140845070431</v>
+      </c>
+      <c r="H38">
+        <v>58</v>
+      </c>
+      <c r="I38">
+        <v>13</v>
+      </c>
+      <c r="J38">
+        <v>4</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="9"/>
+        <v>90</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="10"/>
+        <v>92</v>
+      </c>
+      <c r="M38">
+        <v>23</v>
+      </c>
+      <c r="N38">
+        <v>2</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="4"/>
+        <v>56.521739130434781</v>
+      </c>
+      <c r="R38">
+        <v>13</v>
+      </c>
+      <c r="S38">
+        <v>10</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="6"/>
+        <v>87</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="7"/>
+        <v>95.652173913043484</v>
+      </c>
+      <c r="W38">
+        <v>22</v>
+      </c>
+      <c r="X38">
+        <v>1</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" ref="Y36:Y42" si="11">25-W38-X38</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39">
+        <v>229</v>
+      </c>
+      <c r="E39">
+        <v>99</v>
+      </c>
+      <c r="F39" t="s">
+        <v>119</v>
+      </c>
+      <c r="G39">
+        <v>95.081967213114751</v>
+      </c>
+      <c r="H39">
+        <v>58</v>
+      </c>
+      <c r="I39">
+        <v>3</v>
+      </c>
+      <c r="J39">
+        <v>14</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="9"/>
+        <v>82</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="10"/>
+        <v>91.304347826086953</v>
+      </c>
+      <c r="M39">
+        <v>21</v>
+      </c>
+      <c r="N39">
+        <v>2</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="4"/>
+        <v>95.238095238095227</v>
+      </c>
+      <c r="R39">
+        <v>20</v>
+      </c>
+      <c r="S39">
+        <v>1</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="6"/>
+        <v>68</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="W39">
+        <v>17</v>
+      </c>
+      <c r="X39">
+        <v>0</v>
+      </c>
+      <c r="Y39">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40">
+        <v>255</v>
+      </c>
+      <c r="E40">
+        <v>99</v>
+      </c>
+      <c r="F40" t="s">
+        <v>137</v>
+      </c>
+      <c r="G40">
+        <v>88</v>
+      </c>
+      <c r="H40">
+        <v>66</v>
+      </c>
+      <c r="I40">
+        <v>9</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="9"/>
+        <v>95</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="10"/>
+        <v>96</v>
+      </c>
+      <c r="M40">
+        <v>24</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="4"/>
+        <v>68</v>
+      </c>
+      <c r="R40">
+        <v>17</v>
+      </c>
+      <c r="S40">
+        <v>8</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="W40">
+        <v>25</v>
+      </c>
+      <c r="X40">
+        <v>0</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41">
+        <v>253</v>
+      </c>
+      <c r="G41">
+        <v>95.522388059701484</v>
+      </c>
+      <c r="H41">
+        <v>64</v>
+      </c>
+      <c r="I41">
+        <v>3</v>
+      </c>
+      <c r="J41">
+        <v>8</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="9"/>
+        <v>90</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="10"/>
+        <v>92</v>
+      </c>
+      <c r="M41">
+        <v>23</v>
+      </c>
+      <c r="N41">
+        <v>2</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
+      <c r="R41">
+        <v>19</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="6"/>
+        <v>88</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="W41">
+        <v>22</v>
+      </c>
+      <c r="X41">
+        <v>0</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42">
+        <v>262</v>
+      </c>
+      <c r="G42">
+        <v>91.780821917808225</v>
+      </c>
+      <c r="H42">
+        <v>67</v>
+      </c>
+      <c r="I42">
+        <v>6</v>
+      </c>
+      <c r="J42">
+        <v>2</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="M42">
+        <v>25</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <f t="shared" ref="O36:O42" si="12">25-M42-N42</f>
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <f t="shared" ref="P36:P42" si="13">R42*4-S42</f>
+        <v>67</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="4"/>
+        <v>78.260869565217391</v>
+      </c>
+      <c r="R42">
+        <v>18</v>
+      </c>
+      <c r="S42">
+        <v>5</v>
+      </c>
+      <c r="T42">
+        <f t="shared" ref="T36:T42" si="14">25-R42-S42</f>
+        <v>2</v>
+      </c>
+      <c r="U42">
+        <f t="shared" ref="U36:U42" si="15">W42*4-X42</f>
+        <v>95</v>
+      </c>
+      <c r="V42">
+        <f t="shared" ref="V36:V42" si="16">W42/(W42+X42)*100</f>
+        <v>96</v>
+      </c>
+      <c r="W42">
+        <v>24</v>
+      </c>
+      <c r="X42">
+        <v>1</v>
+      </c>
+      <c r="Y42">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final before jee mains
</commit_message>
<xml_diff>
--- a/Allen_Dark_Analysis.xlsx
+++ b/Allen_Dark_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\CompSciFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B387B40-A68C-49DC-9518-C24FC12FBCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7632135-313F-48E0-8D0D-25669959F663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="152">
   <si>
     <t>Date</t>
   </si>
@@ -233,6 +233,24 @@
     <t>test38.mht</t>
   </si>
   <si>
+    <t>test39.mht</t>
+  </si>
+  <si>
+    <t>test40.mhtml</t>
+  </si>
+  <si>
+    <t>test41.mhtml</t>
+  </si>
+  <si>
+    <t>test42.mhtml</t>
+  </si>
+  <si>
+    <t>test43.mhtml</t>
+  </si>
+  <si>
+    <t>test44.mhtml</t>
+  </si>
+  <si>
     <t>JEE MAINS 24 Jan Shift 1 | 27th Dec,2024 | Online Mode</t>
   </si>
   <si>
@@ -356,6 +374,24 @@
     <t>JEE MAINS 02 April Shift 2 | 1st Jan,1 | Online Mode</t>
   </si>
   <si>
+    <t>JEE MAINS 04 April Shift 1 | 1st Jan,1 | Online Mode</t>
+  </si>
+  <si>
+    <t>JEE MAINS 04 April Shift 2 | 1st Jan,1 | Online Mode</t>
+  </si>
+  <si>
+    <t>JEE MAINS 08 April | 1st Jan,1 | Online Mode</t>
+  </si>
+  <si>
+    <t>JEE MAINS 02 April Shift 2 | 1st Jan,1</t>
+  </si>
+  <si>
+    <t>JEE MAINS 08 Apr Shift 1 | 10th Dec,2024</t>
+  </si>
+  <si>
+    <t>JEE MAINS 08 Apr Shift 2 | 10th Dec,2024</t>
+  </si>
+  <si>
     <t>6015 to 6181</t>
   </si>
   <si>
@@ -447,6 +483,12 @@
   </si>
   <si>
     <t>434 to 457</t>
+  </si>
+  <si>
+    <t>2644 to 2731</t>
+  </si>
+  <si>
+    <t>6955 to 7226</t>
   </si>
 </sst>
 </file>
@@ -788,17 +830,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y42"/>
+  <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
-      <selection activeCell="X41" sqref="X41"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
@@ -894,7 +935,7 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D2">
         <v>193</v>
@@ -903,7 +944,7 @@
         <v>96</v>
       </c>
       <c r="F2" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="G2">
         <v>77.611940298507463</v>
@@ -918,11 +959,9 @@
         <v>8</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K34" si="0">M2*4-N2</f>
         <v>67</v>
       </c>
       <c r="L2">
-        <f t="shared" ref="L2:M34" si="1">M2/(M2+N2)*100</f>
         <v>78.260869565217391</v>
       </c>
       <c r="M2">
@@ -932,15 +971,14 @@
         <v>5</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O41" si="2">25-M2-N2</f>
+        <f>25-M2-N2</f>
         <v>2</v>
       </c>
       <c r="P2">
-        <f t="shared" ref="P2:P41" si="3">R2*4-S2</f>
+        <f>R2*4-S2</f>
         <v>63</v>
       </c>
       <c r="Q2">
-        <f t="shared" ref="Q2:Q42" si="4">R2/(R2+S2)*100</f>
         <v>77.272727272727266</v>
       </c>
       <c r="R2">
@@ -950,15 +988,15 @@
         <v>5</v>
       </c>
       <c r="T2">
-        <f t="shared" ref="T2:T41" si="5">25-R2-S2</f>
+        <f>25-R2-S2</f>
         <v>3</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:U41" si="6">W2*4-X2</f>
+        <f>W2*4-X2</f>
         <v>63</v>
       </c>
       <c r="V2">
-        <f t="shared" ref="V2:V41" si="7">W2/(W2+X2)*100</f>
+        <f>W2/(W2+X2)*100</f>
         <v>77.272727272727266</v>
       </c>
       <c r="W2">
@@ -968,7 +1006,7 @@
         <v>5</v>
       </c>
       <c r="Y2">
-        <f t="shared" ref="Y2:Y37" si="8">25-W2-X2</f>
+        <f>25-W2-X2</f>
         <v>3</v>
       </c>
     </row>
@@ -977,7 +1015,7 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D3">
         <v>178</v>
@@ -986,7 +1024,7 @@
         <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="G3">
         <v>77.41935483870968</v>
@@ -1001,11 +1039,9 @@
         <v>13</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="L3">
-        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="M3">
@@ -1015,15 +1051,14 @@
         <v>2</v>
       </c>
       <c r="O3">
-        <f t="shared" si="2"/>
+        <f>25-M3-N3</f>
         <v>0</v>
       </c>
       <c r="P3">
-        <f t="shared" si="3"/>
+        <f>R3*4-S3</f>
         <v>40</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="R3">
@@ -1033,15 +1068,15 @@
         <v>8</v>
       </c>
       <c r="T3">
-        <f t="shared" si="5"/>
+        <f>25-R3-S3</f>
         <v>5</v>
       </c>
       <c r="U3">
-        <f t="shared" si="6"/>
+        <f>W3*4-X3</f>
         <v>48</v>
       </c>
       <c r="V3">
-        <f t="shared" si="7"/>
+        <f>W3/(W3+X3)*100</f>
         <v>76.470588235294116</v>
       </c>
       <c r="W3">
@@ -1051,7 +1086,7 @@
         <v>4</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="8"/>
+        <f>25-W3-X3</f>
         <v>8</v>
       </c>
     </row>
@@ -1060,7 +1095,7 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D4">
         <v>155</v>
@@ -1069,7 +1104,7 @@
         <v>91</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="G4">
         <v>71.666666666666671</v>
@@ -1084,11 +1119,9 @@
         <v>15</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="L4">
-        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="M4">
@@ -1098,16 +1131,15 @@
         <v>2</v>
       </c>
       <c r="O4">
-        <f t="shared" si="2"/>
+        <f>25-M4-N4</f>
         <v>5</v>
       </c>
       <c r="P4">
-        <f t="shared" si="3"/>
+        <f>R4*4-S4</f>
         <v>44</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="4"/>
-        <v>61.904761904761905</v>
+        <v>61.904761904761912</v>
       </c>
       <c r="R4">
         <v>13</v>
@@ -1116,15 +1148,15 @@
         <v>8</v>
       </c>
       <c r="T4">
-        <f t="shared" si="5"/>
+        <f>25-R4-S4</f>
         <v>4</v>
       </c>
       <c r="U4">
-        <f t="shared" si="6"/>
+        <f>W4*4-X4</f>
         <v>41</v>
       </c>
       <c r="V4">
-        <f t="shared" si="7"/>
+        <f>W4/(W4+X4)*100</f>
         <v>63.157894736842103</v>
       </c>
       <c r="W4">
@@ -1134,7 +1166,7 @@
         <v>7</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="8"/>
+        <f>25-W4-X4</f>
         <v>6</v>
       </c>
     </row>
@@ -1143,7 +1175,7 @@
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D5">
         <v>164</v>
@@ -1152,7 +1184,7 @@
         <v>93</v>
       </c>
       <c r="F5" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="G5">
         <v>69.696969696969703</v>
@@ -1167,11 +1199,9 @@
         <v>9</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="L5">
-        <f t="shared" si="1"/>
         <v>79.166666666666657</v>
       </c>
       <c r="M5">
@@ -1181,15 +1211,14 @@
         <v>5</v>
       </c>
       <c r="O5">
-        <f t="shared" si="2"/>
+        <f>25-M5-N5</f>
         <v>1</v>
       </c>
       <c r="P5">
-        <f t="shared" si="3"/>
+        <f>R5*4-S5</f>
         <v>43</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="4"/>
         <v>59.090909090909093</v>
       </c>
       <c r="R5">
@@ -1199,15 +1228,15 @@
         <v>9</v>
       </c>
       <c r="T5">
-        <f t="shared" si="5"/>
+        <f>25-R5-S5</f>
         <v>3</v>
       </c>
       <c r="U5">
-        <f t="shared" si="6"/>
+        <f>W5*4-X5</f>
         <v>50</v>
       </c>
       <c r="V5">
-        <f t="shared" si="7"/>
+        <f>W5/(W5+X5)*100</f>
         <v>70</v>
       </c>
       <c r="W5">
@@ -1217,7 +1246,7 @@
         <v>6</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="8"/>
+        <f>25-W5-X5</f>
         <v>5</v>
       </c>
     </row>
@@ -1226,7 +1255,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D6">
         <v>222</v>
@@ -1235,7 +1264,7 @@
         <v>98</v>
       </c>
       <c r="F6" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="G6">
         <v>85.294117647058826</v>
@@ -1250,11 +1279,9 @@
         <v>7</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="L6">
-        <f t="shared" si="1"/>
         <v>73.91304347826086</v>
       </c>
       <c r="M6">
@@ -1264,15 +1291,14 @@
         <v>6</v>
       </c>
       <c r="O6">
-        <f t="shared" si="2"/>
+        <f>25-M6-N6</f>
         <v>2</v>
       </c>
       <c r="P6">
-        <f t="shared" si="3"/>
+        <f>R6*4-S6</f>
         <v>78</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="4"/>
         <v>90.909090909090907</v>
       </c>
       <c r="R6">
@@ -1282,15 +1308,15 @@
         <v>2</v>
       </c>
       <c r="T6">
-        <f t="shared" si="5"/>
+        <f>25-R6-S6</f>
         <v>3</v>
       </c>
       <c r="U6">
-        <f t="shared" si="6"/>
+        <f>W6*4-X6</f>
         <v>82</v>
       </c>
       <c r="V6">
-        <f t="shared" si="7"/>
+        <f>W6/(W6+X6)*100</f>
         <v>91.304347826086953</v>
       </c>
       <c r="W6">
@@ -1300,7 +1326,7 @@
         <v>2</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="8"/>
+        <f>25-W6-X6</f>
         <v>2</v>
       </c>
     </row>
@@ -1309,7 +1335,7 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D7">
         <v>210</v>
@@ -1318,7 +1344,7 @@
         <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="G7">
         <v>84.615384615384613</v>
@@ -1333,11 +1359,9 @@
         <v>10</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
         <v>79.166666666666657</v>
       </c>
       <c r="M7">
@@ -1347,15 +1371,14 @@
         <v>5</v>
       </c>
       <c r="O7">
-        <f t="shared" si="2"/>
+        <f>25-M7-N7</f>
         <v>1</v>
       </c>
       <c r="P7">
-        <f t="shared" si="3"/>
+        <f>R7*4-S7</f>
         <v>71</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="4"/>
         <v>79.166666666666657</v>
       </c>
       <c r="R7">
@@ -1365,15 +1388,15 @@
         <v>5</v>
       </c>
       <c r="T7">
-        <f t="shared" si="5"/>
+        <f>25-R7-S7</f>
         <v>1</v>
       </c>
       <c r="U7">
-        <f t="shared" si="6"/>
+        <f>W7*4-X7</f>
         <v>68</v>
       </c>
       <c r="V7">
-        <f t="shared" si="7"/>
+        <f>W7/(W7+X7)*100</f>
         <v>100</v>
       </c>
       <c r="W7">
@@ -1383,7 +1406,7 @@
         <v>0</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="8"/>
+        <f>25-W7-X7</f>
         <v>8</v>
       </c>
     </row>
@@ -1392,7 +1415,7 @@
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D8">
         <v>160</v>
@@ -1401,7 +1424,7 @@
         <v>92</v>
       </c>
       <c r="F8" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="G8">
         <v>73.333333333333329</v>
@@ -1416,11 +1439,9 @@
         <v>15</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
         <v>71.428571428571431</v>
       </c>
       <c r="M8">
@@ -1430,15 +1451,14 @@
         <v>6</v>
       </c>
       <c r="O8">
-        <f t="shared" si="2"/>
+        <f>25-M8-N8</f>
         <v>4</v>
       </c>
       <c r="P8">
-        <f t="shared" si="3"/>
+        <f>R8*4-S8</f>
         <v>64</v>
       </c>
       <c r="Q8">
-        <f>R8/(R8+S8)*100</f>
         <v>80.952380952380949</v>
       </c>
       <c r="R8">
@@ -1448,15 +1468,15 @@
         <v>4</v>
       </c>
       <c r="T8">
-        <f t="shared" si="5"/>
+        <f>25-R8-S8</f>
         <v>4</v>
       </c>
       <c r="U8">
-        <f t="shared" si="6"/>
+        <f>W8*4-X8</f>
         <v>42</v>
       </c>
       <c r="V8">
-        <f t="shared" si="7"/>
+        <f>W8/(W8+X8)*100</f>
         <v>66.666666666666657</v>
       </c>
       <c r="W8">
@@ -1466,7 +1486,7 @@
         <v>6</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="8"/>
+        <f>25-W8-X8</f>
         <v>7</v>
       </c>
     </row>
@@ -1475,7 +1495,7 @@
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D9">
         <v>141</v>
@@ -1484,7 +1504,7 @@
         <v>88</v>
       </c>
       <c r="F9" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="G9">
         <v>67.796610169491515</v>
@@ -1499,11 +1519,9 @@
         <v>16</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="L9">
-        <f t="shared" si="1"/>
         <v>69.565217391304344</v>
       </c>
       <c r="M9">
@@ -1513,15 +1531,14 @@
         <v>7</v>
       </c>
       <c r="O9">
-        <f t="shared" si="2"/>
+        <f>25-M9-N9</f>
         <v>2</v>
       </c>
       <c r="P9">
-        <f t="shared" si="3"/>
+        <f>R9*4-S9</f>
         <v>45</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="R9">
@@ -1531,15 +1548,15 @@
         <v>7</v>
       </c>
       <c r="T9">
-        <f t="shared" si="5"/>
+        <f>25-R9-S9</f>
         <v>5</v>
       </c>
       <c r="U9">
-        <f t="shared" si="6"/>
+        <f>W9*4-X9</f>
         <v>39</v>
       </c>
       <c r="V9">
-        <f t="shared" si="7"/>
+        <f>W9/(W9+X9)*100</f>
         <v>68.75</v>
       </c>
       <c r="W9">
@@ -1549,7 +1566,7 @@
         <v>5</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="8"/>
+        <f>25-W9-X9</f>
         <v>9</v>
       </c>
     </row>
@@ -1558,7 +1575,7 @@
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D10">
         <v>240</v>
@@ -1567,7 +1584,7 @@
         <v>99</v>
       </c>
       <c r="F10" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="G10">
         <v>93.84615384615384</v>
@@ -1582,11 +1599,9 @@
         <v>10</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
         <v>96</v>
       </c>
       <c r="M10">
@@ -1596,15 +1611,14 @@
         <v>1</v>
       </c>
       <c r="O10">
-        <f t="shared" si="2"/>
+        <f>25-M10-N10</f>
         <v>0</v>
       </c>
       <c r="P10">
-        <f t="shared" si="3"/>
+        <f>R10*4-S10</f>
         <v>77</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="4"/>
         <v>86.956521739130437</v>
       </c>
       <c r="R10">
@@ -1614,15 +1628,15 @@
         <v>3</v>
       </c>
       <c r="T10">
-        <f t="shared" si="5"/>
+        <f>25-R10-S10</f>
         <v>2</v>
       </c>
       <c r="U10">
-        <f t="shared" si="6"/>
+        <f>W10*4-X10</f>
         <v>68</v>
       </c>
       <c r="V10">
-        <f t="shared" si="7"/>
+        <f>W10/(W10+X10)*100</f>
         <v>100</v>
       </c>
       <c r="W10">
@@ -1632,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="8"/>
+        <f>25-W10-X10</f>
         <v>8</v>
       </c>
     </row>
@@ -1641,7 +1655,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D11">
         <v>246</v>
@@ -1650,7 +1664,7 @@
         <v>99</v>
       </c>
       <c r="F11" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="G11">
         <v>96.875</v>
@@ -1665,11 +1679,9 @@
         <v>11</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
         <v>96</v>
       </c>
       <c r="L11">
-        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="M11">
@@ -1679,15 +1691,14 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <f t="shared" si="2"/>
+        <f>25-M11-N11</f>
         <v>1</v>
       </c>
       <c r="P11">
-        <f t="shared" si="3"/>
+        <f>R11*4-S11</f>
         <v>96</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="R11">
@@ -1697,15 +1708,15 @@
         <v>0</v>
       </c>
       <c r="T11">
-        <f t="shared" si="5"/>
+        <f>25-R11-S11</f>
         <v>1</v>
       </c>
       <c r="U11">
-        <f t="shared" si="6"/>
+        <f>W11*4-X11</f>
         <v>54</v>
       </c>
       <c r="V11">
-        <f t="shared" si="7"/>
+        <f>W11/(W11+X11)*100</f>
         <v>87.5</v>
       </c>
       <c r="W11">
@@ -1715,7 +1726,7 @@
         <v>2</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="8"/>
+        <f>25-W11-X11</f>
         <v>9</v>
       </c>
     </row>
@@ -1724,7 +1735,7 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D12">
         <v>225</v>
@@ -1733,7 +1744,7 @@
         <v>98</v>
       </c>
       <c r="F12" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="G12">
         <v>95</v>
@@ -1748,11 +1759,9 @@
         <v>15</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
         <v>91</v>
       </c>
       <c r="L12">
-        <f t="shared" si="1"/>
         <v>95.833333333333343</v>
       </c>
       <c r="M12">
@@ -1762,15 +1771,14 @@
         <v>1</v>
       </c>
       <c r="O12">
-        <f t="shared" si="2"/>
+        <f>25-M12-N12</f>
         <v>1</v>
       </c>
       <c r="P12">
-        <f t="shared" si="3"/>
+        <f>R12*4-S12</f>
         <v>67</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="4"/>
         <v>94.444444444444443</v>
       </c>
       <c r="R12">
@@ -1780,15 +1788,15 @@
         <v>1</v>
       </c>
       <c r="T12">
-        <f t="shared" si="5"/>
+        <f>25-R12-S12</f>
         <v>7</v>
       </c>
       <c r="U12">
-        <f t="shared" si="6"/>
+        <f>W12*4-X12</f>
         <v>67</v>
       </c>
       <c r="V12">
-        <f t="shared" si="7"/>
+        <f>W12/(W12+X12)*100</f>
         <v>94.444444444444443</v>
       </c>
       <c r="W12">
@@ -1798,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="8"/>
+        <f>25-W12-X12</f>
         <v>7</v>
       </c>
     </row>
@@ -1807,7 +1815,7 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D13">
         <v>227</v>
@@ -1816,7 +1824,7 @@
         <v>99</v>
       </c>
       <c r="F13" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="G13">
         <v>86.764705882352942</v>
@@ -1831,11 +1839,9 @@
         <v>7</v>
       </c>
       <c r="K13">
-        <f t="shared" si="0"/>
         <v>87</v>
       </c>
       <c r="L13">
-        <f t="shared" si="1"/>
         <v>95.652173913043484</v>
       </c>
       <c r="M13">
@@ -1845,15 +1851,14 @@
         <v>1</v>
       </c>
       <c r="O13">
-        <f t="shared" si="2"/>
+        <f>25-M13-N13</f>
         <v>2</v>
       </c>
       <c r="P13">
-        <f t="shared" si="3"/>
+        <f>R13*4-S13</f>
         <v>76</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="4"/>
         <v>83.333333333333343</v>
       </c>
       <c r="R13">
@@ -1863,15 +1868,15 @@
         <v>4</v>
       </c>
       <c r="T13">
-        <f t="shared" si="5"/>
+        <f>25-R13-S13</f>
         <v>1</v>
       </c>
       <c r="U13">
-        <f t="shared" si="6"/>
+        <f>W13*4-X13</f>
         <v>64</v>
       </c>
       <c r="V13">
-        <f t="shared" si="7"/>
+        <f>W13/(W13+X13)*100</f>
         <v>80.952380952380949</v>
       </c>
       <c r="W13">
@@ -1881,7 +1886,7 @@
         <v>4</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="8"/>
+        <f>25-W13-X13</f>
         <v>4</v>
       </c>
     </row>
@@ -1890,7 +1895,7 @@
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D14">
         <v>229</v>
@@ -1899,7 +1904,7 @@
         <v>99</v>
       </c>
       <c r="F14" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="G14">
         <v>89.393939393939391</v>
@@ -1914,11 +1919,9 @@
         <v>9</v>
       </c>
       <c r="K14">
-        <f t="shared" si="0"/>
         <v>86</v>
       </c>
       <c r="L14">
-        <f t="shared" si="1"/>
         <v>91.666666666666657</v>
       </c>
       <c r="M14">
@@ -1928,15 +1931,14 @@
         <v>2</v>
       </c>
       <c r="O14">
-        <f t="shared" si="2"/>
+        <f>25-M14-N14</f>
         <v>1</v>
       </c>
       <c r="P14">
-        <f t="shared" si="3"/>
+        <f>R14*4-S14</f>
         <v>64</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="4"/>
         <v>80.952380952380949</v>
       </c>
       <c r="R14">
@@ -1946,15 +1948,15 @@
         <v>4</v>
       </c>
       <c r="T14">
-        <f t="shared" si="5"/>
+        <f>25-R14-S14</f>
         <v>4</v>
       </c>
       <c r="U14">
-        <f t="shared" si="6"/>
+        <f>W14*4-X14</f>
         <v>79</v>
       </c>
       <c r="V14">
-        <f t="shared" si="7"/>
+        <f>W14/(W14+X14)*100</f>
         <v>95.238095238095227</v>
       </c>
       <c r="W14">
@@ -1964,7 +1966,7 @@
         <v>1</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="8"/>
+        <f>25-W14-X14</f>
         <v>4</v>
       </c>
     </row>
@@ -1973,7 +1975,7 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D15">
         <v>213</v>
@@ -1982,7 +1984,7 @@
         <v>98</v>
       </c>
       <c r="F15" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="G15">
         <v>88.709677419354833</v>
@@ -1997,11 +1999,9 @@
         <v>13</v>
       </c>
       <c r="K15">
-        <f t="shared" si="0"/>
         <v>86</v>
       </c>
       <c r="L15">
-        <f t="shared" si="1"/>
         <v>91.666666666666657</v>
       </c>
       <c r="M15">
@@ -2011,15 +2011,14 @@
         <v>2</v>
       </c>
       <c r="O15">
-        <f t="shared" si="2"/>
+        <f>25-M15-N15</f>
         <v>1</v>
       </c>
       <c r="P15">
-        <f t="shared" si="3"/>
+        <f>R15*4-S15</f>
         <v>57</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="4"/>
         <v>83.333333333333343</v>
       </c>
       <c r="R15">
@@ -2029,15 +2028,15 @@
         <v>3</v>
       </c>
       <c r="T15">
-        <f t="shared" si="5"/>
+        <f>25-R15-S15</f>
         <v>7</v>
       </c>
       <c r="U15">
-        <f t="shared" si="6"/>
+        <f>W15*4-X15</f>
         <v>70</v>
       </c>
       <c r="V15">
-        <f t="shared" si="7"/>
+        <f>W15/(W15+X15)*100</f>
         <v>90</v>
       </c>
       <c r="W15">
@@ -2047,7 +2046,7 @@
         <v>2</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="8"/>
+        <f>25-W15-X15</f>
         <v>5</v>
       </c>
     </row>
@@ -2056,7 +2055,7 @@
         <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D16">
         <v>208</v>
@@ -2074,11 +2073,9 @@
         <v>23</v>
       </c>
       <c r="K16">
-        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="L16">
-        <f t="shared" si="1"/>
         <v>96</v>
       </c>
       <c r="M16">
@@ -2088,15 +2085,14 @@
         <v>1</v>
       </c>
       <c r="O16">
-        <f t="shared" si="2"/>
+        <f>25-M16-N16</f>
         <v>0</v>
       </c>
       <c r="P16">
-        <f t="shared" si="3"/>
+        <f>R16*4-S16</f>
         <v>60</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="R16">
@@ -2106,15 +2102,15 @@
         <v>4</v>
       </c>
       <c r="T16">
-        <f t="shared" si="5"/>
+        <f>25-R16-S16</f>
         <v>5</v>
       </c>
       <c r="U16">
-        <f t="shared" si="6"/>
+        <f>W16*4-X16</f>
         <v>53</v>
       </c>
       <c r="V16">
-        <f t="shared" si="7"/>
+        <f>W16/(W16+X16)*100</f>
         <v>68.181818181818173</v>
       </c>
       <c r="W16">
@@ -2124,7 +2120,7 @@
         <v>7</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="8"/>
+        <f>25-W16-X16</f>
         <v>3</v>
       </c>
     </row>
@@ -2133,7 +2129,7 @@
         <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D17">
         <v>225</v>
@@ -2151,11 +2147,9 @@
         <v>5</v>
       </c>
       <c r="K17">
-        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="L17">
-        <f t="shared" si="1"/>
         <v>83.333333333333343</v>
       </c>
       <c r="M17">
@@ -2165,15 +2159,14 @@
         <v>4</v>
       </c>
       <c r="O17">
-        <f t="shared" si="2"/>
+        <f>25-M17-N17</f>
         <v>1</v>
       </c>
       <c r="P17">
-        <f t="shared" si="3"/>
+        <f>R17*4-S17</f>
         <v>62</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="4"/>
         <v>73.91304347826086</v>
       </c>
       <c r="R17">
@@ -2183,15 +2176,15 @@
         <v>6</v>
       </c>
       <c r="T17">
-        <f t="shared" si="5"/>
+        <f>25-R17-S17</f>
         <v>2</v>
       </c>
       <c r="U17">
-        <f t="shared" si="6"/>
+        <f>W17*4-X17</f>
         <v>87</v>
       </c>
       <c r="V17">
-        <f t="shared" si="7"/>
+        <f>W17/(W17+X17)*100</f>
         <v>95.652173913043484</v>
       </c>
       <c r="W17">
@@ -2201,7 +2194,7 @@
         <v>1</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="8"/>
+        <f>25-W17-X17</f>
         <v>2</v>
       </c>
     </row>
@@ -2210,7 +2203,7 @@
         <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D18">
         <v>268</v>
@@ -2219,7 +2212,7 @@
         <v>99</v>
       </c>
       <c r="F18" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="G18">
         <v>94.444444444444443</v>
@@ -2234,11 +2227,9 @@
         <v>3</v>
       </c>
       <c r="K18">
-        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="L18">
-        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="M18">
@@ -2248,15 +2239,14 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <f t="shared" si="2"/>
+        <f>25-M18-N18</f>
         <v>0</v>
       </c>
       <c r="P18">
-        <f t="shared" si="3"/>
+        <f>R18*4-S18</f>
         <v>77</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="4"/>
         <v>86.956521739130437</v>
       </c>
       <c r="R18">
@@ -2266,15 +2256,15 @@
         <v>3</v>
       </c>
       <c r="T18">
-        <f t="shared" si="5"/>
+        <f>25-R18-S18</f>
         <v>2</v>
       </c>
       <c r="U18">
-        <f t="shared" si="6"/>
+        <f>W18*4-X18</f>
         <v>91</v>
       </c>
       <c r="V18">
-        <f t="shared" si="7"/>
+        <f>W18/(W18+X18)*100</f>
         <v>95.833333333333343</v>
       </c>
       <c r="W18">
@@ -2284,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="8"/>
+        <f>25-W18-X18</f>
         <v>1</v>
       </c>
     </row>
@@ -2293,7 +2283,7 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D19">
         <v>226</v>
@@ -2302,7 +2292,7 @@
         <v>98</v>
       </c>
       <c r="F19" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="G19">
         <v>85.507246376811594</v>
@@ -2317,11 +2307,9 @@
         <v>6</v>
       </c>
       <c r="K19">
-        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="L19">
-        <f t="shared" si="1"/>
         <v>78.260869565217391</v>
       </c>
       <c r="M19">
@@ -2331,15 +2319,14 @@
         <v>5</v>
       </c>
       <c r="O19">
-        <f t="shared" si="2"/>
+        <f>25-M19-N19</f>
         <v>2</v>
       </c>
       <c r="P19">
-        <f t="shared" si="3"/>
+        <f>R19*4-S19</f>
         <v>86</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="4"/>
         <v>91.666666666666657</v>
       </c>
       <c r="R19">
@@ -2349,15 +2336,15 @@
         <v>2</v>
       </c>
       <c r="T19">
-        <f t="shared" si="5"/>
+        <f>25-R19-S19</f>
         <v>1</v>
       </c>
       <c r="U19">
-        <f t="shared" si="6"/>
+        <f>W19*4-X19</f>
         <v>73</v>
       </c>
       <c r="V19">
-        <f t="shared" si="7"/>
+        <f>W19/(W19+X19)*100</f>
         <v>86.36363636363636</v>
       </c>
       <c r="W19">
@@ -2367,7 +2354,7 @@
         <v>3</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="8"/>
+        <f>25-W19-X19</f>
         <v>3</v>
       </c>
     </row>
@@ -2376,7 +2363,7 @@
         <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D20">
         <v>225</v>
@@ -2385,7 +2372,7 @@
         <v>98</v>
       </c>
       <c r="F20" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="G20">
         <v>84.285714285714292</v>
@@ -2400,11 +2387,9 @@
         <v>5</v>
       </c>
       <c r="K20">
-        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="L20">
-        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="M20">
@@ -2414,15 +2399,14 @@
         <v>5</v>
       </c>
       <c r="O20">
-        <f t="shared" si="2"/>
+        <f>25-M20-N20</f>
         <v>0</v>
       </c>
       <c r="P20">
-        <f t="shared" si="3"/>
+        <f>R20*4-S20</f>
         <v>77</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="4"/>
         <v>86.956521739130437</v>
       </c>
       <c r="R20">
@@ -2432,15 +2416,15 @@
         <v>3</v>
       </c>
       <c r="T20">
-        <f t="shared" si="5"/>
+        <f>25-R20-S20</f>
         <v>2</v>
       </c>
       <c r="U20">
-        <f t="shared" si="6"/>
+        <f>W20*4-X20</f>
         <v>73</v>
       </c>
       <c r="V20">
-        <f t="shared" si="7"/>
+        <f>W20/(W20+X20)*100</f>
         <v>86.36363636363636</v>
       </c>
       <c r="W20">
@@ -2450,7 +2434,7 @@
         <v>3</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="8"/>
+        <f>25-W20-X20</f>
         <v>3</v>
       </c>
     </row>
@@ -2459,7 +2443,7 @@
         <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D21">
         <v>194</v>
@@ -2468,7 +2452,7 @@
         <v>97</v>
       </c>
       <c r="F21" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="G21">
         <v>78.787878787878782</v>
@@ -2483,11 +2467,9 @@
         <v>9</v>
       </c>
       <c r="K21">
-        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="L21">
-        <f t="shared" si="1"/>
         <v>79.166666666666657</v>
       </c>
       <c r="M21">
@@ -2497,15 +2479,14 @@
         <v>5</v>
       </c>
       <c r="O21">
-        <f t="shared" si="2"/>
+        <f>25-M21-N21</f>
         <v>1</v>
       </c>
       <c r="P21">
-        <f t="shared" si="3"/>
+        <f>R21*4-S21</f>
         <v>46</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="4"/>
         <v>68.421052631578945</v>
       </c>
       <c r="R21">
@@ -2515,15 +2496,15 @@
         <v>6</v>
       </c>
       <c r="T21">
-        <f t="shared" si="5"/>
+        <f>25-R21-S21</f>
         <v>6</v>
       </c>
       <c r="U21">
-        <f t="shared" si="6"/>
+        <f>W21*4-X21</f>
         <v>77</v>
       </c>
       <c r="V21">
-        <f t="shared" si="7"/>
+        <f>W21/(W21+X21)*100</f>
         <v>86.956521739130437</v>
       </c>
       <c r="W21">
@@ -2533,7 +2514,7 @@
         <v>3</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="8"/>
+        <f>25-W21-X21</f>
         <v>2</v>
       </c>
     </row>
@@ -2542,7 +2523,7 @@
         <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D22">
         <v>217</v>
@@ -2551,7 +2532,7 @@
         <v>98</v>
       </c>
       <c r="F22" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="G22">
         <v>83.82352941176471</v>
@@ -2566,11 +2547,9 @@
         <v>7</v>
       </c>
       <c r="K22">
-        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="L22">
-        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="M22">
@@ -2580,15 +2559,14 @@
         <v>2</v>
       </c>
       <c r="O22">
-        <f t="shared" si="2"/>
+        <f>25-M22-N22</f>
         <v>0</v>
       </c>
       <c r="P22">
-        <f t="shared" si="3"/>
+        <f>R22*4-S22</f>
         <v>31</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="4"/>
         <v>52.631578947368418</v>
       </c>
       <c r="R22">
@@ -2598,15 +2576,15 @@
         <v>9</v>
       </c>
       <c r="T22">
-        <f t="shared" si="5"/>
+        <f>25-R22-S22</f>
         <v>6</v>
       </c>
       <c r="U22">
-        <f t="shared" si="6"/>
+        <f>W22*4-X22</f>
         <v>96</v>
       </c>
       <c r="V22">
-        <f t="shared" si="7"/>
+        <f>W22/(W22+X22)*100</f>
         <v>100</v>
       </c>
       <c r="W22">
@@ -2616,7 +2594,7 @@
         <v>0</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="8"/>
+        <f>25-W22-X22</f>
         <v>1</v>
       </c>
     </row>
@@ -2625,7 +2603,7 @@
         <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D23">
         <v>233</v>
@@ -2634,7 +2612,7 @@
         <v>99</v>
       </c>
       <c r="F23" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="G23">
         <v>95.161290322580655</v>
@@ -2649,11 +2627,9 @@
         <v>13</v>
       </c>
       <c r="K23">
-        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="L23">
-        <f t="shared" si="1"/>
         <v>86.956521739130437</v>
       </c>
       <c r="M23">
@@ -2663,15 +2639,14 @@
         <v>3</v>
       </c>
       <c r="O23">
-        <f t="shared" si="2"/>
+        <f>25-M23-N23</f>
         <v>2</v>
       </c>
       <c r="P23">
-        <f t="shared" si="3"/>
+        <f>R23*4-S23</f>
         <v>76</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="R23">
@@ -2681,15 +2656,15 @@
         <v>0</v>
       </c>
       <c r="T23">
-        <f t="shared" si="5"/>
+        <f>25-R23-S23</f>
         <v>6</v>
       </c>
       <c r="U23">
-        <f t="shared" si="6"/>
+        <f>W23*4-X23</f>
         <v>80</v>
       </c>
       <c r="V23">
-        <f t="shared" si="7"/>
+        <f>W23/(W23+X23)*100</f>
         <v>100</v>
       </c>
       <c r="W23">
@@ -2699,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="8"/>
+        <f>25-W23-X23</f>
         <v>5</v>
       </c>
     </row>
@@ -2708,7 +2683,7 @@
         <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D24">
         <v>230</v>
@@ -2717,7 +2692,7 @@
         <v>99</v>
       </c>
       <c r="F24" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="G24">
         <v>90.769230769230774</v>
@@ -2732,11 +2707,9 @@
         <v>10</v>
       </c>
       <c r="K24">
-        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="L24">
-        <f t="shared" si="1"/>
         <v>90.476190476190482</v>
       </c>
       <c r="M24">
@@ -2746,15 +2719,14 @@
         <v>2</v>
       </c>
       <c r="O24">
-        <f t="shared" si="2"/>
+        <f>25-M24-N24</f>
         <v>4</v>
       </c>
       <c r="P24">
-        <f t="shared" si="3"/>
+        <f>R24*4-S24</f>
         <v>91</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="4"/>
         <v>95.833333333333343</v>
       </c>
       <c r="R24">
@@ -2764,15 +2736,15 @@
         <v>1</v>
       </c>
       <c r="T24">
-        <f t="shared" si="5"/>
+        <f>25-R24-S24</f>
         <v>1</v>
       </c>
       <c r="U24">
-        <f t="shared" si="6"/>
+        <f>W24*4-X24</f>
         <v>65</v>
       </c>
       <c r="V24">
-        <f t="shared" si="7"/>
+        <f>W24/(W24+X24)*100</f>
         <v>85</v>
       </c>
       <c r="W24">
@@ -2782,7 +2754,7 @@
         <v>3</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="8"/>
+        <f>25-W24-X24</f>
         <v>5</v>
       </c>
     </row>
@@ -2791,7 +2763,7 @@
         <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D25">
         <v>206</v>
@@ -2800,7 +2772,7 @@
         <v>98</v>
       </c>
       <c r="F25" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="G25">
         <v>84.375</v>
@@ -2815,11 +2787,9 @@
         <v>11</v>
       </c>
       <c r="K25">
-        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="L25">
-        <f t="shared" si="1"/>
         <v>87.5</v>
       </c>
       <c r="M25">
@@ -2829,15 +2799,14 @@
         <v>3</v>
       </c>
       <c r="O25">
-        <f t="shared" si="2"/>
+        <f>25-M25-N25</f>
         <v>1</v>
       </c>
       <c r="P25">
-        <f t="shared" si="3"/>
+        <f>R25*4-S25</f>
         <v>59</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="4"/>
         <v>76.19047619047619</v>
       </c>
       <c r="R25">
@@ -2847,15 +2816,15 @@
         <v>5</v>
       </c>
       <c r="T25">
-        <f t="shared" si="5"/>
+        <f>25-R25-S25</f>
         <v>4</v>
       </c>
       <c r="U25">
-        <f t="shared" si="6"/>
+        <f>W25*4-X25</f>
         <v>66</v>
       </c>
       <c r="V25">
-        <f t="shared" si="7"/>
+        <f>W25/(W25+X25)*100</f>
         <v>89.473684210526315</v>
       </c>
       <c r="W25">
@@ -2865,7 +2834,7 @@
         <v>2</v>
       </c>
       <c r="Y25">
-        <f t="shared" si="8"/>
+        <f>25-W25-X25</f>
         <v>6</v>
       </c>
     </row>
@@ -2874,7 +2843,7 @@
         <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D26">
         <v>205</v>
@@ -2883,7 +2852,7 @@
         <v>98</v>
       </c>
       <c r="F26" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="G26">
         <v>78.571428571428569</v>
@@ -2898,11 +2867,9 @@
         <v>5</v>
       </c>
       <c r="K26">
-        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="L26">
-        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="M26">
@@ -2912,15 +2879,14 @@
         <v>6</v>
       </c>
       <c r="O26">
-        <f t="shared" si="2"/>
+        <f>25-M26-N26</f>
         <v>1</v>
       </c>
       <c r="P26">
-        <f t="shared" si="3"/>
+        <f>R26*4-S26</f>
         <v>68</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="4"/>
         <v>81.818181818181827</v>
       </c>
       <c r="R26">
@@ -2930,15 +2896,15 @@
         <v>4</v>
       </c>
       <c r="T26">
-        <f t="shared" si="5"/>
+        <f>25-R26-S26</f>
         <v>3</v>
       </c>
       <c r="U26">
-        <f t="shared" si="6"/>
+        <f>W26*4-X26</f>
         <v>71</v>
       </c>
       <c r="V26">
-        <f t="shared" si="7"/>
+        <f>W26/(W26+X26)*100</f>
         <v>79.166666666666657</v>
       </c>
       <c r="W26">
@@ -2948,7 +2914,7 @@
         <v>5</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="8"/>
+        <f>25-W26-X26</f>
         <v>1</v>
       </c>
     </row>
@@ -2957,7 +2923,7 @@
         <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D27">
         <v>159</v>
@@ -2966,7 +2932,7 @@
         <v>92</v>
       </c>
       <c r="F27" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="G27">
         <v>82.35294117647058</v>
@@ -2981,11 +2947,9 @@
         <v>24</v>
       </c>
       <c r="K27">
-        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="L27">
-        <f t="shared" si="1"/>
         <v>76.19047619047619</v>
       </c>
       <c r="M27">
@@ -2995,15 +2959,14 @@
         <v>5</v>
       </c>
       <c r="O27">
-        <f t="shared" si="2"/>
+        <f>25-M27-N27</f>
         <v>4</v>
       </c>
       <c r="P27">
-        <f t="shared" si="3"/>
+        <f>R27*4-S27</f>
         <v>60</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="R27">
@@ -3013,15 +2976,15 @@
         <v>4</v>
       </c>
       <c r="T27">
-        <f t="shared" si="5"/>
+        <f>25-R27-S27</f>
         <v>5</v>
       </c>
       <c r="U27">
-        <f t="shared" si="6"/>
+        <f>W27*4-X27</f>
         <v>40</v>
       </c>
       <c r="V27">
-        <f t="shared" si="7"/>
+        <f>W27/(W27+X27)*100</f>
         <v>100</v>
       </c>
       <c r="W27">
@@ -3031,7 +2994,7 @@
         <v>0</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="8"/>
+        <f>25-W27-X27</f>
         <v>15</v>
       </c>
     </row>
@@ -3040,7 +3003,7 @@
         <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D28">
         <v>187</v>
@@ -3049,7 +3012,7 @@
         <v>96</v>
       </c>
       <c r="F28" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="G28">
         <v>79.365079365079367</v>
@@ -3064,11 +3027,9 @@
         <v>12</v>
       </c>
       <c r="K28">
-        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="L28">
-        <f t="shared" si="1"/>
         <v>83.333333333333343</v>
       </c>
       <c r="M28">
@@ -3078,15 +3039,14 @@
         <v>4</v>
       </c>
       <c r="O28">
-        <f t="shared" si="2"/>
+        <f>25-M28-N28</f>
         <v>1</v>
       </c>
       <c r="P28">
-        <f t="shared" si="3"/>
+        <f>R28*4-S28</f>
         <v>68</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="4"/>
         <v>81.818181818181827</v>
       </c>
       <c r="R28">
@@ -3096,15 +3056,15 @@
         <v>4</v>
       </c>
       <c r="T28">
-        <f t="shared" si="5"/>
+        <f>25-R28-S28</f>
         <v>3</v>
       </c>
       <c r="U28">
-        <f t="shared" si="6"/>
+        <f>W28*4-X28</f>
         <v>43</v>
       </c>
       <c r="V28">
-        <f t="shared" si="7"/>
+        <f>W28/(W28+X28)*100</f>
         <v>70.588235294117652</v>
       </c>
       <c r="W28">
@@ -3114,7 +3074,7 @@
         <v>5</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="8"/>
+        <f>25-W28-X28</f>
         <v>8</v>
       </c>
     </row>
@@ -3123,7 +3083,7 @@
         <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D29">
         <v>153</v>
@@ -3132,7 +3092,7 @@
         <v>91</v>
       </c>
       <c r="F29" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="G29">
         <v>73.68421052631578</v>
@@ -3147,11 +3107,9 @@
         <v>18</v>
       </c>
       <c r="K29">
-        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="L29">
-        <f t="shared" si="1"/>
         <v>73.91304347826086</v>
       </c>
       <c r="M29">
@@ -3161,15 +3119,14 @@
         <v>6</v>
       </c>
       <c r="O29">
-        <f t="shared" si="2"/>
+        <f>25-M29-N29</f>
         <v>2</v>
       </c>
       <c r="P29">
-        <f t="shared" si="3"/>
+        <f>R29*4-S29</f>
         <v>48</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="4"/>
         <v>76.470588235294116</v>
       </c>
       <c r="R29">
@@ -3179,15 +3136,15 @@
         <v>4</v>
       </c>
       <c r="T29">
-        <f t="shared" si="5"/>
+        <f>25-R29-S29</f>
         <v>8</v>
       </c>
       <c r="U29">
-        <f t="shared" si="6"/>
+        <f>W29*4-X29</f>
         <v>43</v>
       </c>
       <c r="V29">
-        <f t="shared" si="7"/>
+        <f>W29/(W29+X29)*100</f>
         <v>70.588235294117652</v>
       </c>
       <c r="W29">
@@ -3197,7 +3154,7 @@
         <v>5</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="8"/>
+        <f>25-W29-X29</f>
         <v>8</v>
       </c>
     </row>
@@ -3206,7 +3163,7 @@
         <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D30">
         <v>249</v>
@@ -3215,7 +3172,7 @@
         <v>99</v>
       </c>
       <c r="F30" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="G30">
         <v>90.140845070422543</v>
@@ -3230,11 +3187,9 @@
         <v>4</v>
       </c>
       <c r="K30">
-        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="L30">
-        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="M30">
@@ -3244,15 +3199,14 @@
         <v>2</v>
       </c>
       <c r="O30">
-        <f t="shared" si="2"/>
+        <f>25-M30-N30</f>
         <v>0</v>
       </c>
       <c r="P30">
-        <f t="shared" si="3"/>
+        <f>R30*4-S30</f>
         <v>63</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="4"/>
         <v>77.272727272727266</v>
       </c>
       <c r="R30">
@@ -3262,15 +3216,15 @@
         <v>5</v>
       </c>
       <c r="T30">
-        <f t="shared" si="5"/>
+        <f>25-R30-S30</f>
         <v>3</v>
       </c>
       <c r="U30">
-        <f t="shared" si="6"/>
+        <f>W30*4-X30</f>
         <v>96</v>
       </c>
       <c r="V30">
-        <f t="shared" si="7"/>
+        <f>W30/(W30+X30)*100</f>
         <v>100</v>
       </c>
       <c r="W30">
@@ -3280,7 +3234,7 @@
         <v>0</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="8"/>
+        <f>25-W30-X30</f>
         <v>1</v>
       </c>
     </row>
@@ -3289,7 +3243,7 @@
         <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D31">
         <v>171</v>
@@ -3307,11 +3261,9 @@
         <v>6</v>
       </c>
       <c r="K31">
-        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="L31">
-        <f t="shared" si="1"/>
         <v>60.869565217391312</v>
       </c>
       <c r="M31">
@@ -3321,15 +3273,14 @@
         <v>9</v>
       </c>
       <c r="O31">
-        <f t="shared" si="2"/>
+        <f>25-M31-N31</f>
         <v>2</v>
       </c>
       <c r="P31">
-        <f t="shared" si="3"/>
+        <f>R31*4-S31</f>
         <v>37</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="4"/>
         <v>52.173913043478258</v>
       </c>
       <c r="R31">
@@ -3339,15 +3290,15 @@
         <v>11</v>
       </c>
       <c r="T31">
-        <f t="shared" si="5"/>
+        <f>25-R31-S31</f>
         <v>2</v>
       </c>
       <c r="U31">
-        <f t="shared" si="6"/>
+        <f>W31*4-X31</f>
         <v>87</v>
       </c>
       <c r="V31">
-        <f t="shared" si="7"/>
+        <f>W31/(W31+X31)*100</f>
         <v>95.652173913043484</v>
       </c>
       <c r="W31">
@@ -3357,7 +3308,7 @@
         <v>1</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="8"/>
+        <f>25-W31-X31</f>
         <v>2</v>
       </c>
     </row>
@@ -3366,7 +3317,7 @@
         <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D32">
         <v>224</v>
@@ -3384,11 +3335,9 @@
         <v>4</v>
       </c>
       <c r="K32">
-        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="L32">
-        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="M32">
@@ -3398,15 +3347,14 @@
         <v>6</v>
       </c>
       <c r="O32">
-        <f t="shared" si="2"/>
+        <f>25-M32-N32</f>
         <v>1</v>
       </c>
       <c r="P32">
-        <f t="shared" si="3"/>
+        <f>R32*4-S32</f>
         <v>58</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="4"/>
         <v>72.727272727272734</v>
       </c>
       <c r="R32">
@@ -3416,15 +3364,15 @@
         <v>6</v>
       </c>
       <c r="T32">
-        <f t="shared" si="5"/>
+        <f>25-R32-S32</f>
         <v>3</v>
       </c>
       <c r="U32">
-        <f t="shared" si="6"/>
+        <f>W32*4-X32</f>
         <v>100</v>
       </c>
       <c r="V32">
-        <f t="shared" si="7"/>
+        <f>W32/(W32+X32)*100</f>
         <v>100</v>
       </c>
       <c r="W32">
@@ -3434,7 +3382,7 @@
         <v>0</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="8"/>
+        <f>25-W32-X32</f>
         <v>0</v>
       </c>
     </row>
@@ -3443,7 +3391,7 @@
         <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D33">
         <v>157</v>
@@ -3452,7 +3400,7 @@
         <v>91</v>
       </c>
       <c r="F33" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="G33">
         <v>74.137931034482762</v>
@@ -3467,11 +3415,9 @@
         <v>17</v>
       </c>
       <c r="K33">
-        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="L33">
-        <f t="shared" si="1"/>
         <v>72</v>
       </c>
       <c r="M33">
@@ -3481,15 +3427,14 @@
         <v>7</v>
       </c>
       <c r="O33">
-        <f t="shared" si="2"/>
+        <f>25-M33-N33</f>
         <v>0</v>
       </c>
       <c r="P33">
-        <f t="shared" si="3"/>
+        <f>R33*4-S33</f>
         <v>57</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="4"/>
         <v>83.333333333333343</v>
       </c>
       <c r="R33">
@@ -3499,15 +3444,15 @@
         <v>3</v>
       </c>
       <c r="T33">
-        <f t="shared" si="5"/>
+        <f>25-R33-S33</f>
         <v>7</v>
       </c>
       <c r="U33">
-        <f t="shared" si="6"/>
+        <f>W33*4-X33</f>
         <v>35</v>
       </c>
       <c r="V33">
-        <f t="shared" si="7"/>
+        <f>W33/(W33+X33)*100</f>
         <v>66.666666666666657</v>
       </c>
       <c r="W33">
@@ -3517,7 +3462,7 @@
         <v>5</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="8"/>
+        <f>25-W33-X33</f>
         <v>10</v>
       </c>
     </row>
@@ -3526,7 +3471,7 @@
         <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D34">
         <v>192</v>
@@ -3535,7 +3480,7 @@
         <v>96</v>
       </c>
       <c r="F34" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="G34">
         <v>76.470588235294116</v>
@@ -3550,11 +3495,9 @@
         <v>7</v>
       </c>
       <c r="K34">
-        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="L34">
-        <f t="shared" si="1"/>
         <v>62.5</v>
       </c>
       <c r="M34">
@@ -3564,15 +3507,14 @@
         <v>9</v>
       </c>
       <c r="O34">
-        <f t="shared" si="2"/>
+        <f>25-M34-N34</f>
         <v>1</v>
       </c>
       <c r="P34">
-        <f t="shared" si="3"/>
+        <f>R34*4-S34</f>
         <v>53</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="4"/>
         <v>68.181818181818173</v>
       </c>
       <c r="R34">
@@ -3582,15 +3524,15 @@
         <v>7</v>
       </c>
       <c r="T34">
-        <f t="shared" si="5"/>
+        <f>25-R34-S34</f>
         <v>3</v>
       </c>
       <c r="U34">
-        <f t="shared" si="6"/>
+        <f>W34*4-X34</f>
         <v>88</v>
       </c>
       <c r="V34">
-        <f t="shared" si="7"/>
+        <f>W34/(W34+X34)*100</f>
         <v>100</v>
       </c>
       <c r="W34">
@@ -3600,7 +3542,7 @@
         <v>0</v>
       </c>
       <c r="Y34">
-        <f t="shared" si="8"/>
+        <f>25-W34-X34</f>
         <v>3</v>
       </c>
     </row>
@@ -3609,7 +3551,7 @@
         <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D35">
         <v>220</v>
@@ -3627,11 +3569,9 @@
         <v>5</v>
       </c>
       <c r="K35">
-        <f>M35*4-N35</f>
         <v>91</v>
       </c>
       <c r="L35">
-        <f>M35/(M35+N35)*100</f>
         <v>95.833333333333343</v>
       </c>
       <c r="M35">
@@ -3641,15 +3581,14 @@
         <v>1</v>
       </c>
       <c r="O35">
-        <f t="shared" si="2"/>
+        <f>25-M35-N35</f>
         <v>1</v>
       </c>
       <c r="P35">
-        <f t="shared" si="3"/>
+        <f>R35*4-S35</f>
         <v>53</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="4"/>
         <v>68.181818181818173</v>
       </c>
       <c r="R35">
@@ -3659,15 +3598,15 @@
         <v>7</v>
       </c>
       <c r="T35">
-        <f t="shared" si="5"/>
+        <f>25-R35-S35</f>
         <v>3</v>
       </c>
       <c r="U35">
-        <f t="shared" si="6"/>
+        <f>W35*4-X35</f>
         <v>76</v>
       </c>
       <c r="V35">
-        <f t="shared" si="7"/>
+        <f>W35/(W35+X35)*100</f>
         <v>83.333333333333343</v>
       </c>
       <c r="W35">
@@ -3677,7 +3616,7 @@
         <v>4</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="8"/>
+        <f>25-W35-X35</f>
         <v>1</v>
       </c>
     </row>
@@ -3686,7 +3625,7 @@
         <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D36">
         <v>183</v>
@@ -3704,11 +3643,9 @@
         <v>8</v>
       </c>
       <c r="K36">
-        <f t="shared" ref="K36:K42" si="9">M36*4-N36</f>
         <v>68</v>
       </c>
       <c r="L36">
-        <f t="shared" ref="L36:M42" si="10">M36/(M36+N36)*100</f>
         <v>81.818181818181827</v>
       </c>
       <c r="M36">
@@ -3718,15 +3655,14 @@
         <v>4</v>
       </c>
       <c r="O36">
-        <f t="shared" si="2"/>
+        <f>25-M36-N36</f>
         <v>3</v>
       </c>
       <c r="P36">
-        <f t="shared" si="3"/>
+        <f>R36*4-S36</f>
         <v>38</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="4"/>
         <v>54.54545454545454</v>
       </c>
       <c r="R36">
@@ -3736,15 +3672,15 @@
         <v>10</v>
       </c>
       <c r="T36">
-        <f t="shared" si="5"/>
+        <f>25-R36-S36</f>
         <v>3</v>
       </c>
       <c r="U36">
-        <f t="shared" si="6"/>
+        <f>W36*4-X36</f>
         <v>78</v>
       </c>
       <c r="V36">
-        <f t="shared" si="7"/>
+        <f>W36/(W36+X36)*100</f>
         <v>90.909090909090907</v>
       </c>
       <c r="W36">
@@ -3754,7 +3690,7 @@
         <v>2</v>
       </c>
       <c r="Y36">
-        <f t="shared" si="8"/>
+        <f>25-W36-X36</f>
         <v>3</v>
       </c>
     </row>
@@ -3763,7 +3699,7 @@
         <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D37">
         <v>211</v>
@@ -3772,7 +3708,7 @@
         <v>98</v>
       </c>
       <c r="F37" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="G37">
         <v>81.159420289855078</v>
@@ -3787,11 +3723,9 @@
         <v>6</v>
       </c>
       <c r="K37">
-        <f t="shared" si="9"/>
         <v>80</v>
       </c>
       <c r="L37">
-        <f t="shared" si="10"/>
         <v>84</v>
       </c>
       <c r="M37">
@@ -3801,15 +3735,14 @@
         <v>4</v>
       </c>
       <c r="O37">
-        <f t="shared" si="2"/>
+        <f>25-M37-N37</f>
         <v>0</v>
       </c>
       <c r="P37">
-        <f t="shared" si="3"/>
+        <f>R37*4-S37</f>
         <v>74</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="4"/>
         <v>90.476190476190482</v>
       </c>
       <c r="R37">
@@ -3819,15 +3752,15 @@
         <v>2</v>
       </c>
       <c r="T37">
-        <f t="shared" si="5"/>
+        <f>25-R37-S37</f>
         <v>4</v>
       </c>
       <c r="U37">
-        <f t="shared" si="6"/>
+        <f>W37*4-X37</f>
         <v>57</v>
       </c>
       <c r="V37">
-        <f t="shared" si="7"/>
+        <f>W37/(W37+X37)*100</f>
         <v>69.565217391304344</v>
       </c>
       <c r="W37">
@@ -3837,7 +3770,7 @@
         <v>7</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="8"/>
+        <f>25-W37-X37</f>
         <v>2</v>
       </c>
     </row>
@@ -3846,7 +3779,7 @@
         <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D38">
         <v>219</v>
@@ -3855,7 +3788,7 @@
         <v>98</v>
       </c>
       <c r="F38" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="G38">
         <v>81.690140845070431</v>
@@ -3870,11 +3803,9 @@
         <v>4</v>
       </c>
       <c r="K38">
-        <f t="shared" si="9"/>
         <v>90</v>
       </c>
       <c r="L38">
-        <f t="shared" si="10"/>
         <v>92</v>
       </c>
       <c r="M38">
@@ -3884,15 +3815,14 @@
         <v>2</v>
       </c>
       <c r="O38">
-        <f t="shared" si="2"/>
+        <f>25-M38-N38</f>
         <v>0</v>
       </c>
       <c r="P38">
-        <f t="shared" si="3"/>
+        <f>R38*4-S38</f>
         <v>42</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="4"/>
         <v>56.521739130434781</v>
       </c>
       <c r="R38">
@@ -3902,15 +3832,15 @@
         <v>10</v>
       </c>
       <c r="T38">
-        <f t="shared" si="5"/>
+        <f>25-R38-S38</f>
         <v>2</v>
       </c>
       <c r="U38">
-        <f t="shared" si="6"/>
+        <f>W38*4-X38</f>
         <v>87</v>
       </c>
       <c r="V38">
-        <f t="shared" si="7"/>
+        <f>W38/(W38+X38)*100</f>
         <v>95.652173913043484</v>
       </c>
       <c r="W38">
@@ -3920,7 +3850,7 @@
         <v>1</v>
       </c>
       <c r="Y38">
-        <f t="shared" ref="Y36:Y42" si="11">25-W38-X38</f>
+        <f>25-W38-X38</f>
         <v>2</v>
       </c>
     </row>
@@ -3929,7 +3859,7 @@
         <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D39">
         <v>229</v>
@@ -3938,7 +3868,7 @@
         <v>99</v>
       </c>
       <c r="F39" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="G39">
         <v>95.081967213114751</v>
@@ -3953,11 +3883,9 @@
         <v>14</v>
       </c>
       <c r="K39">
-        <f t="shared" si="9"/>
         <v>82</v>
       </c>
       <c r="L39">
-        <f t="shared" si="10"/>
         <v>91.304347826086953</v>
       </c>
       <c r="M39">
@@ -3967,15 +3895,14 @@
         <v>2</v>
       </c>
       <c r="O39">
-        <f t="shared" si="2"/>
+        <f>25-M39-N39</f>
         <v>2</v>
       </c>
       <c r="P39">
-        <f t="shared" si="3"/>
+        <f>R39*4-S39</f>
         <v>79</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="4"/>
         <v>95.238095238095227</v>
       </c>
       <c r="R39">
@@ -3985,15 +3912,15 @@
         <v>1</v>
       </c>
       <c r="T39">
-        <f t="shared" si="5"/>
+        <f>25-R39-S39</f>
         <v>4</v>
       </c>
       <c r="U39">
-        <f t="shared" si="6"/>
+        <f>W39*4-X39</f>
         <v>68</v>
       </c>
       <c r="V39">
-        <f t="shared" si="7"/>
+        <f>W39/(W39+X39)*100</f>
         <v>100</v>
       </c>
       <c r="W39">
@@ -4003,7 +3930,7 @@
         <v>0</v>
       </c>
       <c r="Y39">
-        <f t="shared" si="11"/>
+        <f>25-W39-X39</f>
         <v>8</v>
       </c>
     </row>
@@ -4012,7 +3939,7 @@
         <v>63</v>
       </c>
       <c r="C40" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D40">
         <v>255</v>
@@ -4021,7 +3948,7 @@
         <v>99</v>
       </c>
       <c r="F40" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="G40">
         <v>88</v>
@@ -4036,11 +3963,9 @@
         <v>0</v>
       </c>
       <c r="K40">
-        <f t="shared" si="9"/>
         <v>95</v>
       </c>
       <c r="L40">
-        <f t="shared" si="10"/>
         <v>96</v>
       </c>
       <c r="M40">
@@ -4050,15 +3975,14 @@
         <v>1</v>
       </c>
       <c r="O40">
-        <f t="shared" si="2"/>
+        <f>25-M40-N40</f>
         <v>0</v>
       </c>
       <c r="P40">
-        <f t="shared" si="3"/>
+        <f>R40*4-S40</f>
         <v>60</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="R40">
@@ -4068,15 +3992,15 @@
         <v>8</v>
       </c>
       <c r="T40">
-        <f t="shared" si="5"/>
+        <f>25-R40-S40</f>
         <v>0</v>
       </c>
       <c r="U40">
-        <f t="shared" si="6"/>
+        <f>W40*4-X40</f>
         <v>100</v>
       </c>
       <c r="V40">
-        <f t="shared" si="7"/>
+        <f>W40/(W40+X40)*100</f>
         <v>100</v>
       </c>
       <c r="W40">
@@ -4086,7 +4010,7 @@
         <v>0</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="11"/>
+        <f>25-W40-X40</f>
         <v>0</v>
       </c>
     </row>
@@ -4095,7 +4019,7 @@
         <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="D41">
         <v>253</v>
@@ -4113,11 +4037,9 @@
         <v>8</v>
       </c>
       <c r="K41">
-        <f t="shared" si="9"/>
         <v>90</v>
       </c>
       <c r="L41">
-        <f t="shared" si="10"/>
         <v>92</v>
       </c>
       <c r="M41">
@@ -4127,15 +4049,14 @@
         <v>2</v>
       </c>
       <c r="O41">
-        <f t="shared" si="2"/>
+        <f>25-M41-N41</f>
         <v>0</v>
       </c>
       <c r="P41">
-        <f t="shared" si="3"/>
+        <f>R41*4-S41</f>
         <v>75</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="4"/>
         <v>95</v>
       </c>
       <c r="R41">
@@ -4145,15 +4066,15 @@
         <v>1</v>
       </c>
       <c r="T41">
-        <f t="shared" si="5"/>
+        <f>25-R41-S41</f>
         <v>5</v>
       </c>
       <c r="U41">
-        <f t="shared" si="6"/>
+        <f>W41*4-X41</f>
         <v>88</v>
       </c>
       <c r="V41">
-        <f t="shared" si="7"/>
+        <f>W41/(W41+X41)*100</f>
         <v>100</v>
       </c>
       <c r="W41">
@@ -4163,7 +4084,7 @@
         <v>0</v>
       </c>
       <c r="Y41">
-        <f t="shared" si="11"/>
+        <f>25-W41-X41</f>
         <v>3</v>
       </c>
     </row>
@@ -4172,7 +4093,7 @@
         <v>65</v>
       </c>
       <c r="C42" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D42">
         <v>262</v>
@@ -4190,11 +4111,9 @@
         <v>2</v>
       </c>
       <c r="K42">
-        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="L42">
-        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="M42">
@@ -4204,15 +4123,14 @@
         <v>0</v>
       </c>
       <c r="O42">
-        <f t="shared" ref="O36:O42" si="12">25-M42-N42</f>
+        <f>25-M42-N42</f>
         <v>0</v>
       </c>
       <c r="P42">
-        <f t="shared" ref="P36:P42" si="13">R42*4-S42</f>
+        <f>R42*4-S42</f>
         <v>67</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="4"/>
         <v>78.260869565217391</v>
       </c>
       <c r="R42">
@@ -4222,15 +4140,15 @@
         <v>5</v>
       </c>
       <c r="T42">
-        <f t="shared" ref="T36:T42" si="14">25-R42-S42</f>
+        <f>25-R42-S42</f>
         <v>2</v>
       </c>
       <c r="U42">
-        <f t="shared" ref="U36:U42" si="15">W42*4-X42</f>
+        <f>W42*4-X42</f>
         <v>95</v>
       </c>
       <c r="V42">
-        <f t="shared" ref="V36:V42" si="16">W42/(W42+X42)*100</f>
+        <f>W42/(W42+X42)*100</f>
         <v>96</v>
       </c>
       <c r="W42">
@@ -4240,12 +4158,474 @@
         <v>1</v>
       </c>
       <c r="Y42">
-        <f t="shared" si="11"/>
+        <f>25-W42-X42</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43">
+        <v>259</v>
+      </c>
+      <c r="G43">
+        <v>92.957746478873233</v>
+      </c>
+      <c r="H43">
+        <v>66</v>
+      </c>
+      <c r="I43">
+        <v>5</v>
+      </c>
+      <c r="J43">
+        <v>4</v>
+      </c>
+      <c r="K43">
+        <v>85</v>
+      </c>
+      <c r="L43">
+        <v>88</v>
+      </c>
+      <c r="M43">
+        <v>22</v>
+      </c>
+      <c r="N43">
+        <v>3</v>
+      </c>
+      <c r="O43">
+        <f>25-M43-N43</f>
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <f>R43*4-S43</f>
+        <v>74</v>
+      </c>
+      <c r="Q43">
+        <v>90.476190476190482</v>
+      </c>
+      <c r="R43">
+        <v>19</v>
+      </c>
+      <c r="S43">
+        <v>2</v>
+      </c>
+      <c r="T43">
+        <f>25-R43-S43</f>
+        <v>4</v>
+      </c>
+      <c r="U43">
+        <f>W43*4-X43</f>
+        <v>100</v>
+      </c>
+      <c r="V43">
+        <f>W43/(W43+X43)*100</f>
+        <v>100</v>
+      </c>
+      <c r="W43">
+        <v>25</v>
+      </c>
+      <c r="X43">
+        <v>0</v>
+      </c>
+      <c r="Y43">
+        <f>25-W43-X43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44">
+        <v>251</v>
+      </c>
+      <c r="G44">
+        <v>98.4375</v>
+      </c>
+      <c r="H44">
+        <v>63</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>11</v>
+      </c>
+      <c r="K44">
+        <v>95</v>
+      </c>
+      <c r="L44">
+        <v>96</v>
+      </c>
+      <c r="M44">
+        <v>24</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+      <c r="O44">
+        <f>25-M44-N44</f>
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <f>R44*4-S44</f>
+        <v>68</v>
+      </c>
+      <c r="Q44">
+        <v>100</v>
+      </c>
+      <c r="R44">
+        <v>17</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="T44">
+        <f>25-R44-S44</f>
+        <v>8</v>
+      </c>
+      <c r="U44">
+        <f>W44*4-X44</f>
+        <v>88</v>
+      </c>
+      <c r="V44">
+        <f>W44/(W44+X44)*100</f>
+        <v>100</v>
+      </c>
+      <c r="W44">
+        <v>22</v>
+      </c>
+      <c r="X44">
+        <v>0</v>
+      </c>
+      <c r="Y44">
+        <f>25-W44-X44</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" t="s">
+        <v>115</v>
+      </c>
+      <c r="D45">
+        <v>257</v>
+      </c>
+      <c r="G45">
+        <v>95.588235294117652</v>
+      </c>
+      <c r="H45">
+        <v>65</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>7</v>
+      </c>
+      <c r="K45">
+        <v>100</v>
+      </c>
+      <c r="L45">
+        <v>100</v>
+      </c>
+      <c r="M45">
+        <v>25</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <f>25-M45-N45</f>
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <f>R45*4-S45</f>
+        <v>62</v>
+      </c>
+      <c r="Q45">
+        <v>88.888888888888886</v>
+      </c>
+      <c r="R45">
+        <v>16</v>
+      </c>
+      <c r="S45">
+        <v>2</v>
+      </c>
+      <c r="T45">
+        <f>25-R45-S45</f>
+        <v>7</v>
+      </c>
+      <c r="U45">
+        <f>W45*4-X45</f>
+        <v>95</v>
+      </c>
+      <c r="V45">
+        <f>W45/(W45+X45)*100</f>
+        <v>96</v>
+      </c>
+      <c r="W45">
+        <v>24</v>
+      </c>
+      <c r="X45">
+        <v>1</v>
+      </c>
+      <c r="Y45">
+        <f>25-W45-X45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46">
+        <v>256</v>
+      </c>
+      <c r="G46">
+        <v>94.20289855072464</v>
+      </c>
+      <c r="H46">
+        <v>65</v>
+      </c>
+      <c r="I46">
+        <v>4</v>
+      </c>
+      <c r="J46">
+        <v>6</v>
+      </c>
+      <c r="K46">
+        <v>90</v>
+      </c>
+      <c r="L46">
+        <v>92</v>
+      </c>
+      <c r="M46">
+        <v>23</v>
+      </c>
+      <c r="N46">
+        <v>2</v>
+      </c>
+      <c r="O46">
+        <f>25-M46-N46</f>
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <f>R46*4-S46</f>
+        <v>82</v>
+      </c>
+      <c r="Q46">
+        <v>91.304347826086953</v>
+      </c>
+      <c r="R46">
+        <v>21</v>
+      </c>
+      <c r="S46">
+        <v>2</v>
+      </c>
+      <c r="T46">
+        <f>25-R46-S46</f>
+        <v>2</v>
+      </c>
+      <c r="U46">
+        <f>W46*4-X46</f>
+        <v>84</v>
+      </c>
+      <c r="V46">
+        <f>W46/(W46+X46)*100</f>
+        <v>100</v>
+      </c>
+      <c r="W46">
+        <v>21</v>
+      </c>
+      <c r="X46">
+        <v>0</v>
+      </c>
+      <c r="Y46">
+        <f>25-W46-X46</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" t="s">
+        <v>117</v>
+      </c>
+      <c r="D47">
+        <v>216</v>
+      </c>
+      <c r="E47">
+        <v>98</v>
+      </c>
+      <c r="F47" t="s">
+        <v>150</v>
+      </c>
+      <c r="G47">
+        <v>82.608695652173907</v>
+      </c>
+      <c r="H47">
+        <v>57</v>
+      </c>
+      <c r="I47">
+        <v>12</v>
+      </c>
+      <c r="J47">
+        <v>6</v>
+      </c>
+      <c r="K47">
+        <f>M47*4-N47</f>
+        <v>62</v>
+      </c>
+      <c r="L47">
+        <f>M47*100/(M47+N47)</f>
+        <v>73.913043478260875</v>
+      </c>
+      <c r="M47">
+        <v>17</v>
+      </c>
+      <c r="N47">
+        <v>6</v>
+      </c>
+      <c r="O47">
+        <f>25-M47-N47</f>
+        <v>2</v>
+      </c>
+      <c r="P47">
+        <f>R47*4-S47</f>
+        <v>86</v>
+      </c>
+      <c r="Q47">
+        <f>R47*100/(R47+S47)</f>
+        <v>91.666666666666671</v>
+      </c>
+      <c r="R47">
+        <v>22</v>
+      </c>
+      <c r="S47">
+        <v>2</v>
+      </c>
+      <c r="T47">
+        <f>25-R47-S47</f>
+        <v>1</v>
+      </c>
+      <c r="U47">
+        <f>W47*4-X47</f>
+        <v>68</v>
+      </c>
+      <c r="V47">
+        <f>W47/(W47+X47)*100</f>
+        <v>81.818181818181827</v>
+      </c>
+      <c r="W47">
+        <v>18</v>
+      </c>
+      <c r="X47">
+        <v>4</v>
+      </c>
+      <c r="Y47">
+        <f>25-W47-X47</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D48">
+        <v>188</v>
+      </c>
+      <c r="E48">
+        <v>96</v>
+      </c>
+      <c r="F48" t="s">
+        <v>151</v>
+      </c>
+      <c r="G48">
+        <v>72.222222222222214</v>
+      </c>
+      <c r="H48">
+        <v>52</v>
+      </c>
+      <c r="I48">
+        <v>20</v>
+      </c>
+      <c r="J48">
+        <v>3</v>
+      </c>
+      <c r="K48">
+        <f>M48*4-N48</f>
+        <v>55</v>
+      </c>
+      <c r="L48">
+        <f>M48*100/(M48+N48)</f>
+        <v>64</v>
+      </c>
+      <c r="M48">
+        <v>16</v>
+      </c>
+      <c r="N48">
+        <v>9</v>
+      </c>
+      <c r="O48">
+        <f>25-M48-N48</f>
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <f>R48*4-S48</f>
+        <v>46</v>
+      </c>
+      <c r="Q48">
+        <f>R48*100/(R48+S48)</f>
+        <v>58.333333333333336</v>
+      </c>
+      <c r="R48">
+        <v>14</v>
+      </c>
+      <c r="S48">
+        <v>10</v>
+      </c>
+      <c r="T48">
+        <f>25-R48-S48</f>
+        <v>1</v>
+      </c>
+      <c r="U48">
+        <f>W48*4-X48</f>
+        <v>87</v>
+      </c>
+      <c r="V48">
+        <f>W48/(W48+X48)*100</f>
+        <v>95.652173913043484</v>
+      </c>
+      <c r="W48">
+        <v>22</v>
+      </c>
+      <c r="X48">
+        <v>1</v>
+      </c>
+      <c r="Y48">
+        <f>25-W48-X48</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D42">
+  <conditionalFormatting sqref="D2:D48">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4257,7 +4637,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E42">
+  <conditionalFormatting sqref="E2:E48">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4269,7 +4649,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G42">
+  <conditionalFormatting sqref="G2:G48">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -4281,7 +4661,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H42">
+  <conditionalFormatting sqref="H2:H48">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -4293,7 +4673,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I42">
+  <conditionalFormatting sqref="I2:I48">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -4305,7 +4685,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K42">
+  <conditionalFormatting sqref="K2:K48">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -4317,7 +4697,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L42">
+  <conditionalFormatting sqref="L2:L48">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -4329,7 +4709,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M42">
+  <conditionalFormatting sqref="M2:M48">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -4341,7 +4721,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N42">
+  <conditionalFormatting sqref="N2:N48">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -4353,7 +4733,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P42">
+  <conditionalFormatting sqref="P2:P48">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -4365,7 +4745,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q42">
+  <conditionalFormatting sqref="Q2:Q48">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -4377,7 +4757,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R42">
+  <conditionalFormatting sqref="R2:R48">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -4389,7 +4769,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S42">
+  <conditionalFormatting sqref="S2:S48">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -4401,7 +4781,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U42">
+  <conditionalFormatting sqref="U2:U48">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -4413,7 +4793,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V42">
+  <conditionalFormatting sqref="V2:V48">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -4425,7 +4805,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W42">
+  <conditionalFormatting sqref="W2:W48">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -4437,7 +4817,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X42">
+  <conditionalFormatting sqref="X2:X48">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>